<commit_message>
【更新】2020/10 月營收 / 2020Q3 EPS
</commit_message>
<xml_diff>
--- a/all_stock.xlsx
+++ b/all_stock.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\download\rich_stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3A15C2-BD53-466B-A59E-73DA168839E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AF14CA-C090-41B6-BCFA-F5B55BFA807C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_stock" sheetId="1" r:id="rId1"/>
-    <sheet name="config" sheetId="2" r:id="rId2"/>
+    <sheet name="資訊列表" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5326" uniqueCount="1822">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5354" uniqueCount="1849">
   <si>
     <t>代碼</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -5580,6 +5580,114 @@
   <si>
     <t>買入價
 可估</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>location</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>priceHigh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buyPrice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sellPrice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>股本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>淨值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>netInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QEPS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020Q3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EPS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>毛利率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>營業利益率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>稅前淨利率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>稅後淨利率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>月營收</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>年度/月份</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>月增</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>年増</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>累計營收</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>累計年增</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020/10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Single Stock</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5627,7 +5735,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -5635,11 +5743,128 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5663,6 +5888,45 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -5945,7 +6209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1749"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
@@ -30934,13 +31198,174 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00A392A-89DF-4573-A544-23CF075C2A72}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="10" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="10" t="s">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="10" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="11" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>1833</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="11" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="12" t="s">
+        <v>1834</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>1835</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="15"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="17" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="15"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="17" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="15"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="18"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20" t="s">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="12" t="s">
+        <v>1841</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>1847</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="15"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="17" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="15"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17" t="s">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="15"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="17" t="s">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="18"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="20" t="s">
+        <v>1846</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1. 修正 id (name) -> name(id) 2. 新增營收顯示總值
</commit_message>
<xml_diff>
--- a/all_stock.xlsx
+++ b/all_stock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\download\rich_stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DDADCC-638E-41FE-94B5-671D216FE4D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A402108F-844A-4BAB-BAB7-55859516CA17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="180" windowWidth="21150" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_stock" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5645" uniqueCount="1952">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5638" uniqueCount="1950">
   <si>
     <t>代碼</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -5380,31 +5380,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>定存股,傳產</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>定存股,傳產,水資源</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>定存股,食品</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>傳產</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>食品</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>綠能</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TESLA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -5446,11 +5422,6 @@
   </si>
   <si>
     <t>台積電</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>博奕
-長線</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -5986,12 +5957,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>核心
-車用
-Teals</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>電腦選
 矽晶圓</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6147,6 +6112,38 @@
   </si>
   <si>
     <t>電機機械</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DDR5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DRAM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>房室回溫
+2020 營收沒衰退</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>博奕
+長線
+月營收 7.5E
+單月EPS 5塊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>核心
+Tesla</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9月 EPS 0.9
+10月 EPS 1.08
+11月營收新高
+2021 EPS上看15塊</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -6672,8 +6669,8 @@
   <dimension ref="A1:L1747"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I103" sqref="I103"/>
+      <pane ySplit="1" topLeftCell="A1100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1109" sqref="K1109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6687,7 +6684,7 @@
     <col min="7" max="7" width="8.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="8.140625" style="2" customWidth="1"/>
     <col min="10" max="10" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" style="7" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" style="7" customWidth="1"/>
     <col min="12" max="12" width="48.42578125" style="5" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -6706,22 +6703,22 @@
         <v>1771</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>1942</v>
+        <v>1934</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>1854</v>
+        <v>1847</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>1812</v>
+        <v>1805</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>1860</v>
+        <v>1853</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>1794</v>
+        <v>1787</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>1793</v>
+        <v>1786</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>1765</v>
@@ -6730,7 +6727,7 @@
         <v>1764</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1101</v>
       </c>
@@ -6744,16 +6741,16 @@
         <v>988</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>1862</v>
+        <v>1855</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>1849</v>
+        <v>1842</v>
       </c>
       <c r="G2" s="2">
         <v>41</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>1775</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -6769,9 +6766,6 @@
       <c r="D3" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="K3" s="7" t="s">
-        <v>1775</v>
-      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -6786,9 +6780,6 @@
       <c r="D4" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="K4" s="7" t="s">
-        <v>1778</v>
-      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -6803,11 +6794,8 @@
       <c r="D5" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>1775</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1108</v>
       </c>
@@ -6819,9 +6807,6 @@
       </c>
       <c r="D6" s="2" t="s">
         <v>988</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>1776</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -6879,9 +6864,6 @@
       <c r="D10" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="K10" s="7" t="s">
-        <v>1779</v>
-      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -6896,9 +6878,6 @@
       <c r="D11" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="K11" s="7" t="s">
-        <v>1777</v>
-      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -6927,9 +6906,6 @@
       <c r="D13" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="K13" s="7" t="s">
-        <v>1777</v>
-      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -6944,9 +6920,6 @@
       <c r="D14" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="K14" s="7" t="s">
-        <v>1777</v>
-      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -6967,7 +6940,7 @@
         <v>1218</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1898</v>
+        <v>1891</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>4</v>
@@ -6976,7 +6949,7 @@
         <v>988</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>1943</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -7007,7 +6980,7 @@
         <v>988</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>1943</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -7080,7 +7053,7 @@
         <v>988</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>1944</v>
+        <v>1936</v>
       </c>
       <c r="G23" s="2">
         <v>100</v>
@@ -7425,10 +7398,10 @@
         <v>988</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>1936</v>
+        <v>1928</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>1853</v>
+        <v>1846</v>
       </c>
       <c r="H47" s="2">
         <v>120</v>
@@ -7546,16 +7519,16 @@
         <v>988</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>1945</v>
+        <v>1937</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>1849</v>
+        <v>1842</v>
       </c>
       <c r="G55" s="2">
         <v>9.5</v>
       </c>
       <c r="K55" s="7" t="s">
-        <v>1803</v>
+        <v>1796</v>
       </c>
       <c r="L55" s="5" t="s">
         <v>1774</v>
@@ -8070,7 +8043,7 @@
         <v>1466</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>1787</v>
+        <v>1781</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>4</v>
@@ -8079,16 +8052,16 @@
         <v>988</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>1933</v>
+        <v>1925</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>1855</v>
+        <v>1848</v>
       </c>
       <c r="H92" s="2">
         <v>20</v>
       </c>
       <c r="K92" s="7" t="s">
-        <v>1856</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
@@ -8245,7 +8218,7 @@
         <v>988</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>1951</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.25">
@@ -8262,7 +8235,7 @@
         <v>988</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>1951</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.25">
@@ -8293,13 +8266,13 @@
         <v>988</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>1946</v>
+        <v>1938</v>
       </c>
       <c r="G106" s="2">
         <v>50</v>
       </c>
       <c r="L106" s="5" t="s">
-        <v>1947</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.25">
@@ -8330,17 +8303,17 @@
         <v>988</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>1948</v>
+        <v>1940</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>1857</v>
+        <v>1850</v>
       </c>
       <c r="G108" s="2">
         <v>46</v>
       </c>
       <c r="K108" s="5"/>
       <c r="L108" s="5" t="s">
-        <v>1858</v>
+        <v>1851</v>
       </c>
     </row>
     <row r="109" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -8357,7 +8330,7 @@
         <v>988</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>1946</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.25">
@@ -8374,7 +8347,7 @@
         <v>988</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>1866</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.25">
@@ -8405,7 +8378,7 @@
         <v>988</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>1927</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -8492,7 +8465,7 @@
         <v>988</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>1927</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -8593,7 +8566,7 @@
         <v>988</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>1914</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -8792,7 +8765,7 @@
         <v>988</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>1850</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="140" spans="1:12" x14ac:dyDescent="0.25">
@@ -8837,16 +8810,16 @@
         <v>988</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>1866</v>
+        <v>1859</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>1855</v>
+        <v>1848</v>
       </c>
       <c r="G142" s="2">
         <v>110</v>
       </c>
       <c r="L142" s="5" t="s">
-        <v>1905</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="143" spans="1:12" x14ac:dyDescent="0.25">
@@ -9213,7 +9186,7 @@
         <v>988</v>
       </c>
       <c r="E168" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -10098,7 +10071,7 @@
         <v>988</v>
       </c>
       <c r="E231" s="2" t="s">
-        <v>1868</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
@@ -10255,7 +10228,7 @@
         <v>988</v>
       </c>
       <c r="E242" s="2" t="s">
-        <v>1934</v>
+        <v>1926</v>
       </c>
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.25">
@@ -10314,7 +10287,7 @@
         <v>988</v>
       </c>
       <c r="E246" s="2" t="s">
-        <v>1906</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.25">
@@ -10331,7 +10304,7 @@
         <v>988</v>
       </c>
       <c r="E247" s="2" t="s">
-        <v>1906</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.25">
@@ -10362,7 +10335,7 @@
         <v>988</v>
       </c>
       <c r="E249" s="2" t="s">
-        <v>1907</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="250" spans="1:12" x14ac:dyDescent="0.25">
@@ -10393,7 +10366,7 @@
         <v>988</v>
       </c>
       <c r="E251" s="2" t="s">
-        <v>1906</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.25">
@@ -10424,19 +10397,19 @@
         <v>988</v>
       </c>
       <c r="E253" s="2" t="s">
-        <v>1914</v>
+        <v>1907</v>
       </c>
       <c r="F253" s="2" t="s">
-        <v>1857</v>
+        <v>1850</v>
       </c>
       <c r="G253" s="2">
         <v>160</v>
       </c>
       <c r="K253" s="7" t="s">
-        <v>1804</v>
+        <v>1797</v>
       </c>
       <c r="L253" s="5" t="s">
-        <v>1795</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.25">
@@ -10551,10 +10524,10 @@
         <v>988</v>
       </c>
       <c r="E261" s="4" t="s">
-        <v>1918</v>
+        <v>1910</v>
       </c>
       <c r="F261" s="2" t="s">
-        <v>1849</v>
+        <v>1842</v>
       </c>
       <c r="G261" s="2">
         <v>35</v>
@@ -10588,7 +10561,7 @@
         <v>988</v>
       </c>
       <c r="E263" s="2" t="s">
-        <v>1850</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.25">
@@ -10619,7 +10592,7 @@
         <v>988</v>
       </c>
       <c r="E265" s="2" t="s">
-        <v>1864</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.25">
@@ -10664,7 +10637,7 @@
         <v>988</v>
       </c>
       <c r="E268" s="2" t="s">
-        <v>1922</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.25">
@@ -10723,7 +10696,7 @@
         <v>988</v>
       </c>
       <c r="E272" s="2" t="s">
-        <v>1863</v>
+        <v>1856</v>
       </c>
       <c r="G272" s="2">
         <v>420</v>
@@ -10771,7 +10744,7 @@
         <v>988</v>
       </c>
       <c r="E275" s="4" t="s">
-        <v>1917</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
@@ -10886,7 +10859,7 @@
         <v>988</v>
       </c>
       <c r="E283" s="2" t="s">
-        <v>1938</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
@@ -10903,7 +10876,7 @@
         <v>988</v>
       </c>
       <c r="E284" s="2" t="s">
-        <v>1937</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
@@ -10976,7 +10949,7 @@
         <v>988</v>
       </c>
       <c r="E289" s="2" t="s">
-        <v>1848</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
@@ -11035,7 +11008,7 @@
         <v>988</v>
       </c>
       <c r="E293" s="2" t="s">
-        <v>1848</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
@@ -11164,7 +11137,7 @@
         <v>988</v>
       </c>
       <c r="E302" s="2" t="s">
-        <v>1864</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
@@ -11195,7 +11168,7 @@
         <v>988</v>
       </c>
       <c r="E304" s="2" t="s">
-        <v>1928</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="305" spans="1:12" x14ac:dyDescent="0.25">
@@ -11231,7 +11204,7 @@
         <v>2375</v>
       </c>
       <c r="B307" s="1" t="s">
-        <v>1784</v>
+        <v>1778</v>
       </c>
       <c r="C307" s="2" t="s">
         <v>4</v>
@@ -11240,19 +11213,19 @@
         <v>988</v>
       </c>
       <c r="E307" s="4" t="s">
-        <v>1872</v>
+        <v>1865</v>
       </c>
       <c r="F307" s="2" t="s">
-        <v>1859</v>
+        <v>1852</v>
       </c>
       <c r="G307" s="2">
         <v>60</v>
       </c>
       <c r="K307" s="7" t="s">
-        <v>1785</v>
+        <v>1779</v>
       </c>
       <c r="L307" s="5" t="s">
-        <v>1796</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="308" spans="1:12" x14ac:dyDescent="0.25">
@@ -11283,7 +11256,7 @@
         <v>988</v>
       </c>
       <c r="L309" s="5" t="s">
-        <v>1809</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="310" spans="1:12" x14ac:dyDescent="0.25">
@@ -11300,7 +11273,7 @@
         <v>988</v>
       </c>
       <c r="E310" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="311" spans="1:12" x14ac:dyDescent="0.25">
@@ -11373,7 +11346,7 @@
         <v>988</v>
       </c>
       <c r="E315" s="2" t="s">
-        <v>1897</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="316" spans="1:12" x14ac:dyDescent="0.25">
@@ -11575,7 +11548,7 @@
         <v>988</v>
       </c>
       <c r="E329" s="2" t="s">
-        <v>1923</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="330" spans="1:12" x14ac:dyDescent="0.25">
@@ -11592,7 +11565,7 @@
         <v>988</v>
       </c>
       <c r="E330" s="2" t="s">
-        <v>1920</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="331" spans="1:12" x14ac:dyDescent="0.25">
@@ -11623,13 +11596,13 @@
         <v>988</v>
       </c>
       <c r="E332" s="2" t="s">
-        <v>1848</v>
+        <v>1841</v>
       </c>
       <c r="F332" s="2" t="s">
-        <v>1849</v>
+        <v>1842</v>
       </c>
       <c r="L332" s="5" t="s">
-        <v>1900</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="333" spans="1:12" x14ac:dyDescent="0.25">
@@ -11660,10 +11633,10 @@
         <v>988</v>
       </c>
       <c r="E334" s="2" t="s">
-        <v>1848</v>
+        <v>1841</v>
       </c>
       <c r="F334" s="2" t="s">
-        <v>1853</v>
+        <v>1846</v>
       </c>
       <c r="H334" s="2">
         <v>60</v>
@@ -11711,7 +11684,7 @@
         <v>988</v>
       </c>
       <c r="E337" s="2" t="s">
-        <v>1879</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.25">
@@ -11826,7 +11799,7 @@
         <v>988</v>
       </c>
       <c r="E345" s="2" t="s">
-        <v>1937</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.25">
@@ -11941,7 +11914,7 @@
         <v>988</v>
       </c>
       <c r="E353" s="2" t="s">
-        <v>1902</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="354" spans="1:7" x14ac:dyDescent="0.25">
@@ -12000,7 +11973,7 @@
         <v>988</v>
       </c>
       <c r="E357" s="2" t="s">
-        <v>1882</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="358" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -12017,10 +11990,10 @@
         <v>988</v>
       </c>
       <c r="E358" s="4" t="s">
-        <v>1871</v>
+        <v>1864</v>
       </c>
       <c r="F358" s="2" t="s">
-        <v>1849</v>
+        <v>1842</v>
       </c>
       <c r="G358" s="2">
         <v>32</v>
@@ -12082,7 +12055,7 @@
         <v>988</v>
       </c>
       <c r="E362" s="4" t="s">
-        <v>1941</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="363" spans="1:7" x14ac:dyDescent="0.25">
@@ -12113,7 +12086,7 @@
         <v>988</v>
       </c>
       <c r="E364" s="2" t="s">
-        <v>1863</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="365" spans="1:7" x14ac:dyDescent="0.25">
@@ -12144,7 +12117,7 @@
         <v>988</v>
       </c>
       <c r="E366" s="2" t="s">
-        <v>1897</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="367" spans="1:7" x14ac:dyDescent="0.25">
@@ -12301,7 +12274,7 @@
         <v>988</v>
       </c>
       <c r="E377" s="2" t="s">
-        <v>1930</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="378" spans="1:12" x14ac:dyDescent="0.25">
@@ -12360,7 +12333,7 @@
         <v>988</v>
       </c>
       <c r="E381" s="2" t="s">
-        <v>1863</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="382" spans="1:12" x14ac:dyDescent="0.25">
@@ -12391,13 +12364,13 @@
         <v>988</v>
       </c>
       <c r="E383" s="2" t="s">
-        <v>1863</v>
+        <v>1856</v>
       </c>
       <c r="I383" s="2">
         <v>46.6</v>
       </c>
       <c r="L383" s="5" t="s">
-        <v>1901</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="384" spans="1:12" x14ac:dyDescent="0.25">
@@ -12470,7 +12443,7 @@
         <v>988</v>
       </c>
       <c r="E388" s="2" t="s">
-        <v>1897</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="389" spans="1:11" x14ac:dyDescent="0.25">
@@ -12529,16 +12502,16 @@
         <v>988</v>
       </c>
       <c r="E392" s="4" t="s">
-        <v>1870</v>
+        <v>1863</v>
       </c>
       <c r="F392" s="2" t="s">
-        <v>1859</v>
+        <v>1852</v>
       </c>
       <c r="G392" s="2">
         <v>190</v>
       </c>
       <c r="K392" s="7" t="s">
-        <v>1852</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="393" spans="1:11" x14ac:dyDescent="0.25">
@@ -12597,7 +12570,7 @@
         <v>988</v>
       </c>
       <c r="E396" s="2" t="s">
-        <v>1914</v>
+        <v>1907</v>
       </c>
     </row>
     <row r="397" spans="1:11" x14ac:dyDescent="0.25">
@@ -12754,7 +12727,7 @@
         <v>988</v>
       </c>
       <c r="E407" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.25">
@@ -12967,10 +12940,10 @@
         <v>988</v>
       </c>
       <c r="E422" s="2" t="s">
-        <v>1862</v>
+        <v>1855</v>
       </c>
       <c r="F422" s="2" t="s">
-        <v>1849</v>
+        <v>1842</v>
       </c>
       <c r="G422" s="2">
         <v>46</v>
@@ -13536,16 +13509,16 @@
         <v>988</v>
       </c>
       <c r="E462" s="4" t="s">
-        <v>1899</v>
+        <v>1892</v>
       </c>
       <c r="F462" s="2" t="s">
-        <v>1849</v>
+        <v>1842</v>
       </c>
       <c r="G462" s="2">
         <v>32</v>
       </c>
       <c r="K462" s="7" t="s">
-        <v>1803</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="463" spans="1:11" x14ac:dyDescent="0.25">
@@ -13800,19 +13773,19 @@
         <v>988</v>
       </c>
       <c r="E480" s="4" t="s">
-        <v>1899</v>
+        <v>1892</v>
       </c>
       <c r="F480" s="2" t="s">
-        <v>1861</v>
+        <v>1854</v>
       </c>
       <c r="G480" s="2">
         <v>15.5</v>
       </c>
       <c r="K480" s="7" t="s">
-        <v>1802</v>
+        <v>1795</v>
       </c>
       <c r="L480" s="5" t="s">
-        <v>1798</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="481" spans="1:12" x14ac:dyDescent="0.25">
@@ -13829,7 +13802,7 @@
         <v>988</v>
       </c>
       <c r="E481" s="2" t="s">
-        <v>1899</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="482" spans="1:12" x14ac:dyDescent="0.25">
@@ -13874,19 +13847,19 @@
         <v>988</v>
       </c>
       <c r="E484" s="4" t="s">
-        <v>1899</v>
+        <v>1892</v>
       </c>
       <c r="F484" s="2" t="s">
-        <v>1861</v>
+        <v>1854</v>
       </c>
       <c r="G484" s="2">
         <v>30</v>
       </c>
       <c r="K484" s="7" t="s">
-        <v>1802</v>
+        <v>1795</v>
       </c>
       <c r="L484" s="5" t="s">
-        <v>1800</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="485" spans="1:12" x14ac:dyDescent="0.25">
@@ -13945,19 +13918,19 @@
         <v>988</v>
       </c>
       <c r="E488" s="4" t="s">
-        <v>1899</v>
+        <v>1892</v>
       </c>
       <c r="F488" s="2" t="s">
-        <v>1861</v>
+        <v>1854</v>
       </c>
       <c r="G488" s="2">
         <v>20</v>
       </c>
       <c r="K488" s="7" t="s">
-        <v>1802</v>
+        <v>1795</v>
       </c>
       <c r="L488" s="5" t="s">
-        <v>1801</v>
+        <v>1794</v>
       </c>
     </row>
     <row r="489" spans="1:12" x14ac:dyDescent="0.25">
@@ -13974,19 +13947,19 @@
         <v>988</v>
       </c>
       <c r="E489" s="4" t="s">
-        <v>1899</v>
+        <v>1892</v>
       </c>
       <c r="F489" s="2" t="s">
-        <v>1861</v>
+        <v>1854</v>
       </c>
       <c r="G489" s="2">
         <v>14</v>
       </c>
       <c r="K489" s="7" t="s">
-        <v>1802</v>
+        <v>1795</v>
       </c>
       <c r="L489" s="5" t="s">
-        <v>1788</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="490" spans="1:12" x14ac:dyDescent="0.25">
@@ -14003,19 +13976,19 @@
         <v>988</v>
       </c>
       <c r="E490" s="4" t="s">
-        <v>1899</v>
+        <v>1892</v>
       </c>
       <c r="F490" s="2" t="s">
-        <v>1861</v>
+        <v>1854</v>
       </c>
       <c r="G490" s="2">
         <v>23.5</v>
       </c>
       <c r="K490" s="7" t="s">
-        <v>1802</v>
+        <v>1795</v>
       </c>
       <c r="L490" s="5" t="s">
-        <v>1799</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="491" spans="1:12" x14ac:dyDescent="0.25">
@@ -14256,7 +14229,7 @@
         <v>988</v>
       </c>
       <c r="E507" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.25">
@@ -14329,7 +14302,7 @@
         <v>988</v>
       </c>
       <c r="E512" s="2" t="s">
-        <v>1890</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="513" spans="1:11" x14ac:dyDescent="0.25">
@@ -14346,7 +14319,7 @@
         <v>988</v>
       </c>
       <c r="E513" s="2" t="s">
-        <v>1890</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="514" spans="1:11" x14ac:dyDescent="0.25">
@@ -14503,16 +14476,16 @@
         <v>988</v>
       </c>
       <c r="E524" s="4" t="s">
-        <v>1876</v>
+        <v>1869</v>
       </c>
       <c r="F524" s="2" t="s">
-        <v>1859</v>
+        <v>1852</v>
       </c>
       <c r="G524" s="2">
         <v>55</v>
       </c>
       <c r="K524" s="7" t="s">
-        <v>1865</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="525" spans="1:11" x14ac:dyDescent="0.25">
@@ -14529,7 +14502,7 @@
         <v>988</v>
       </c>
       <c r="E525" s="2" t="s">
-        <v>1949</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="526" spans="1:11" x14ac:dyDescent="0.25">
@@ -14588,7 +14561,7 @@
         <v>988</v>
       </c>
       <c r="E529" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="530" spans="1:5" x14ac:dyDescent="0.25">
@@ -14605,7 +14578,7 @@
         <v>988</v>
       </c>
       <c r="E530" s="2" t="s">
-        <v>1879</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="531" spans="1:5" x14ac:dyDescent="0.25">
@@ -14636,7 +14609,7 @@
         <v>988</v>
       </c>
       <c r="E532" s="2" t="s">
-        <v>1786</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="533" spans="1:5" x14ac:dyDescent="0.25">
@@ -14667,7 +14640,7 @@
         <v>988</v>
       </c>
       <c r="E534" s="2" t="s">
-        <v>1881</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="535" spans="1:5" x14ac:dyDescent="0.25">
@@ -14712,7 +14685,7 @@
         <v>988</v>
       </c>
       <c r="E537" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="538" spans="1:5" x14ac:dyDescent="0.25">
@@ -14771,7 +14744,7 @@
         <v>988</v>
       </c>
       <c r="E541" s="2" t="s">
-        <v>1879</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="542" spans="1:5" x14ac:dyDescent="0.25">
@@ -14802,7 +14775,7 @@
         <v>988</v>
       </c>
       <c r="E543" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="544" spans="1:5" x14ac:dyDescent="0.25">
@@ -14875,7 +14848,7 @@
         <v>988</v>
       </c>
       <c r="E548" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="549" spans="1:12" x14ac:dyDescent="0.25">
@@ -14920,10 +14893,10 @@
         <v>988</v>
       </c>
       <c r="E551" s="2" t="s">
-        <v>1864</v>
+        <v>1857</v>
       </c>
       <c r="F551" s="2" t="s">
-        <v>1859</v>
+        <v>1852</v>
       </c>
       <c r="G551" s="2">
         <v>78</v>
@@ -14971,16 +14944,16 @@
         <v>988</v>
       </c>
       <c r="E554" s="4" t="s">
-        <v>1878</v>
+        <v>1871</v>
       </c>
       <c r="F554" s="2" t="s">
-        <v>1857</v>
+        <v>1850</v>
       </c>
       <c r="G554" s="2">
         <v>29</v>
       </c>
       <c r="L554" s="5" t="s">
-        <v>1805</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="555" spans="1:12" x14ac:dyDescent="0.25">
@@ -15039,7 +15012,7 @@
         <v>988</v>
       </c>
       <c r="E558" s="2" t="s">
-        <v>1920</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="559" spans="1:12" x14ac:dyDescent="0.25">
@@ -15336,7 +15309,7 @@
         <v>988</v>
       </c>
       <c r="E579" s="2" t="s">
-        <v>1864</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.25">
@@ -15591,7 +15564,7 @@
         <v>988</v>
       </c>
       <c r="E597" s="2" t="s">
-        <v>1949</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="598" spans="1:5" x14ac:dyDescent="0.25">
@@ -15720,7 +15693,7 @@
         <v>988</v>
       </c>
       <c r="E606" s="2" t="s">
-        <v>1924</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="607" spans="1:5" x14ac:dyDescent="0.25">
@@ -15779,7 +15752,7 @@
         <v>988</v>
       </c>
       <c r="E610" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="611" spans="1:11" x14ac:dyDescent="0.25">
@@ -15855,7 +15828,7 @@
         <v>988</v>
       </c>
       <c r="E615" s="4" t="s">
-        <v>1939</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="616" spans="1:11" x14ac:dyDescent="0.25">
@@ -15970,7 +15943,7 @@
         <v>988</v>
       </c>
       <c r="K623" s="7" t="s">
-        <v>1780</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="624" spans="1:11" x14ac:dyDescent="0.25">
@@ -16127,7 +16100,7 @@
         <v>988</v>
       </c>
       <c r="E634" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="635" spans="1:8" x14ac:dyDescent="0.25">
@@ -16144,7 +16117,7 @@
         <v>988</v>
       </c>
       <c r="E635" s="2" t="s">
-        <v>1867</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="636" spans="1:8" x14ac:dyDescent="0.25">
@@ -16175,10 +16148,10 @@
         <v>988</v>
       </c>
       <c r="E637" s="2" t="s">
+        <v>1841</v>
+      </c>
+      <c r="F637" s="2" t="s">
         <v>1848</v>
-      </c>
-      <c r="F637" s="2" t="s">
-        <v>1855</v>
       </c>
       <c r="H637" s="2">
         <v>100</v>
@@ -16226,7 +16199,7 @@
         <v>988</v>
       </c>
       <c r="E640" s="2" t="s">
-        <v>1920</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="641" spans="1:5" x14ac:dyDescent="0.25">
@@ -16299,7 +16272,7 @@
         <v>988</v>
       </c>
       <c r="E645" s="2" t="s">
-        <v>1937</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="646" spans="1:5" x14ac:dyDescent="0.25">
@@ -16386,7 +16359,7 @@
         <v>988</v>
       </c>
       <c r="E651" s="2" t="s">
-        <v>1850</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="652" spans="1:5" x14ac:dyDescent="0.25">
@@ -16473,7 +16446,7 @@
         <v>988</v>
       </c>
       <c r="E657" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
       <c r="G657" s="2">
         <v>115</v>
@@ -16717,10 +16690,10 @@
         <v>988</v>
       </c>
       <c r="E674" s="4" t="s">
-        <v>1873</v>
+        <v>1866</v>
       </c>
       <c r="F674" s="2" t="s">
-        <v>1857</v>
+        <v>1850</v>
       </c>
       <c r="G674" s="2">
         <v>45</v>
@@ -17076,7 +17049,7 @@
         <v>988</v>
       </c>
       <c r="E699" s="2" t="s">
-        <v>1920</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="700" spans="1:5" x14ac:dyDescent="0.25">
@@ -17149,7 +17122,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="705" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="705" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A705" s="3">
         <v>4927</v>
       </c>
@@ -17163,7 +17136,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="706" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="706" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A706" s="3">
         <v>4930</v>
       </c>
@@ -17177,7 +17150,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="707" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="707" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A707" s="3">
         <v>4934</v>
       </c>
@@ -17191,10 +17164,10 @@
         <v>988</v>
       </c>
       <c r="E707" s="2" t="s">
-        <v>1783</v>
-      </c>
-    </row>
-    <row r="708" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1777</v>
+      </c>
+    </row>
+    <row r="708" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A708" s="3">
         <v>4935</v>
       </c>
@@ -17208,7 +17181,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="709" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="709" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A709" s="3">
         <v>4938</v>
       </c>
@@ -17222,7 +17195,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="710" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="710" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A710" s="3">
         <v>4942</v>
       </c>
@@ -17236,7 +17209,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="711" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="711" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A711" s="3">
         <v>4943</v>
       </c>
@@ -17250,7 +17223,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="712" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="712" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A712" s="3">
         <v>4952</v>
       </c>
@@ -17264,7 +17237,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="713" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="713" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A713" s="3">
         <v>4956</v>
       </c>
@@ -17278,7 +17251,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="714" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="714" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A714" s="3">
         <v>4958</v>
       </c>
@@ -17292,7 +17265,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="715" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="715" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A715" s="3">
         <v>4960</v>
       </c>
@@ -17306,7 +17279,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="716" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="716" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A716" s="3">
         <v>4961</v>
       </c>
@@ -17320,10 +17293,10 @@
         <v>988</v>
       </c>
       <c r="E716" s="2" t="s">
-        <v>1922</v>
-      </c>
-    </row>
-    <row r="717" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1914</v>
+      </c>
+    </row>
+    <row r="717" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A717" s="3">
         <v>4967</v>
       </c>
@@ -17336,11 +17309,14 @@
       <c r="D717" s="2" t="s">
         <v>988</v>
       </c>
-      <c r="E717" s="2" t="s">
-        <v>1897</v>
-      </c>
-    </row>
-    <row r="718" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E717" s="4" t="s">
+        <v>1945</v>
+      </c>
+      <c r="L717" s="5" t="s">
+        <v>1944</v>
+      </c>
+    </row>
+    <row r="718" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A718" s="3">
         <v>4968</v>
       </c>
@@ -17354,10 +17330,10 @@
         <v>988</v>
       </c>
       <c r="E718" s="2" t="s">
-        <v>1894</v>
-      </c>
-    </row>
-    <row r="719" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1887</v>
+      </c>
+    </row>
+    <row r="719" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A719" s="3">
         <v>4976</v>
       </c>
@@ -17371,10 +17347,10 @@
         <v>988</v>
       </c>
       <c r="E719" s="2" t="s">
-        <v>1949</v>
-      </c>
-    </row>
-    <row r="720" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="720" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A720" s="3">
         <v>4977</v>
       </c>
@@ -17416,7 +17392,7 @@
         <v>988</v>
       </c>
       <c r="E722" s="2" t="s">
-        <v>1888</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="723" spans="1:12" x14ac:dyDescent="0.25">
@@ -17475,19 +17451,19 @@
         <v>988</v>
       </c>
       <c r="E726" s="2" t="s">
+        <v>1841</v>
+      </c>
+      <c r="F726" s="2" t="s">
         <v>1848</v>
-      </c>
-      <c r="F726" s="2" t="s">
-        <v>1855</v>
       </c>
       <c r="H726" s="2">
         <v>160</v>
       </c>
       <c r="K726" s="7" t="s">
-        <v>1806</v>
+        <v>1799</v>
       </c>
       <c r="L726" s="5" t="s">
-        <v>1807</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="727" spans="1:12" x14ac:dyDescent="0.25">
@@ -17913,10 +17889,10 @@
         <v>988</v>
       </c>
       <c r="E756" s="4" t="s">
-        <v>1929</v>
+        <v>1921</v>
       </c>
       <c r="F756" s="2" t="s">
-        <v>1849</v>
+        <v>1842</v>
       </c>
       <c r="G756" s="2">
         <v>130</v>
@@ -18048,7 +18024,7 @@
         <v>988</v>
       </c>
       <c r="E765" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="766" spans="1:7" x14ac:dyDescent="0.25">
@@ -18079,7 +18055,7 @@
         <v>988</v>
       </c>
       <c r="E767" s="2" t="s">
-        <v>1924</v>
+        <v>1916</v>
       </c>
     </row>
     <row r="768" spans="1:7" x14ac:dyDescent="0.25">
@@ -18222,7 +18198,7 @@
         <v>988</v>
       </c>
       <c r="E777" s="4" t="s">
-        <v>1875</v>
+        <v>1868</v>
       </c>
       <c r="G777" s="2">
         <v>34</v>
@@ -18354,13 +18330,13 @@
         <v>988</v>
       </c>
       <c r="E786" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
       <c r="G786" s="2">
         <v>45</v>
       </c>
       <c r="L786" s="5" t="s">
-        <v>1895</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="787" spans="1:12" x14ac:dyDescent="0.25">
@@ -18405,7 +18381,7 @@
         <v>988</v>
       </c>
       <c r="E789" s="2" t="s">
-        <v>1864</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="790" spans="1:12" x14ac:dyDescent="0.25">
@@ -18492,7 +18468,7 @@
         <v>988</v>
       </c>
       <c r="E795" s="4" t="s">
-        <v>1877</v>
+        <v>1870</v>
       </c>
       <c r="G795" s="2">
         <v>42</v>
@@ -18526,7 +18502,7 @@
         <v>988</v>
       </c>
       <c r="E797" s="2" t="s">
-        <v>1949</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="798" spans="1:12" x14ac:dyDescent="0.25">
@@ -18711,7 +18687,7 @@
         <v>988</v>
       </c>
       <c r="E810" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="811" spans="1:12" x14ac:dyDescent="0.25">
@@ -18742,10 +18718,10 @@
         <v>988</v>
       </c>
       <c r="E812" s="2" t="s">
-        <v>1902</v>
+        <v>1895</v>
       </c>
       <c r="L812" s="5" t="s">
-        <v>1903</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="813" spans="1:12" x14ac:dyDescent="0.25">
@@ -18776,7 +18752,7 @@
         <v>988</v>
       </c>
       <c r="E814" s="2" t="s">
-        <v>1897</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="815" spans="1:12" x14ac:dyDescent="0.25">
@@ -18793,7 +18769,7 @@
         <v>988</v>
       </c>
       <c r="E815" s="2" t="s">
-        <v>1937</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="816" spans="1:12" x14ac:dyDescent="0.25">
@@ -18838,7 +18814,7 @@
         <v>988</v>
       </c>
       <c r="E818" s="2" t="s">
-        <v>1897</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="819" spans="1:7" x14ac:dyDescent="0.25">
@@ -18939,7 +18915,7 @@
         <v>988</v>
       </c>
       <c r="E825" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="826" spans="1:7" x14ac:dyDescent="0.25">
@@ -18998,10 +18974,10 @@
         <v>988</v>
       </c>
       <c r="E829" s="4" t="s">
-        <v>1783</v>
+        <v>1777</v>
       </c>
       <c r="F829" s="2" t="s">
-        <v>1859</v>
+        <v>1852</v>
       </c>
       <c r="G829" s="2">
         <v>30</v>
@@ -19259,10 +19235,10 @@
         <v>988</v>
       </c>
       <c r="E847" s="2" t="s">
-        <v>1934</v>
+        <v>1926</v>
       </c>
       <c r="F847" s="2" t="s">
-        <v>1855</v>
+        <v>1848</v>
       </c>
       <c r="H847" s="2">
         <v>190</v>
@@ -19282,7 +19258,7 @@
         <v>988</v>
       </c>
       <c r="E848" s="2" t="s">
-        <v>1786</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="849" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
@@ -19299,7 +19275,7 @@
         <v>988</v>
       </c>
       <c r="E849" s="4" t="s">
-        <v>1929</v>
+        <v>1921</v>
       </c>
       <c r="G849" s="2">
         <v>65</v>
@@ -19417,7 +19393,7 @@
         <v>988</v>
       </c>
       <c r="E857" s="2" t="s">
-        <v>1904</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="858" spans="1:7" x14ac:dyDescent="0.25">
@@ -19504,7 +19480,7 @@
         <v>988</v>
       </c>
       <c r="E863" s="2" t="s">
-        <v>1883</v>
+        <v>1876</v>
       </c>
       <c r="G863" s="2">
         <v>140</v>
@@ -19580,16 +19556,16 @@
         <v>988</v>
       </c>
       <c r="E868" s="4" t="s">
-        <v>1912</v>
+        <v>1905</v>
       </c>
       <c r="F868" s="2" t="s">
-        <v>1859</v>
+        <v>1852</v>
       </c>
       <c r="G868" s="2">
         <v>25</v>
       </c>
       <c r="L868" s="8" t="s">
-        <v>1808</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="869" spans="1:12" x14ac:dyDescent="0.25">
@@ -19606,10 +19582,10 @@
         <v>988</v>
       </c>
       <c r="E869" s="2" t="s">
-        <v>1930</v>
+        <v>1922</v>
       </c>
       <c r="L869" s="5" t="s">
-        <v>1931</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="870" spans="1:12" x14ac:dyDescent="0.25">
@@ -19654,7 +19630,7 @@
         <v>988</v>
       </c>
       <c r="E872" s="2" t="s">
-        <v>1864</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="873" spans="1:12" x14ac:dyDescent="0.25">
@@ -19699,7 +19675,7 @@
         <v>988</v>
       </c>
       <c r="E875" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="876" spans="1:12" x14ac:dyDescent="0.25">
@@ -19721,7 +19697,7 @@
         <v>8103</v>
       </c>
       <c r="B877" s="1" t="s">
-        <v>1932</v>
+        <v>1924</v>
       </c>
       <c r="C877" s="2" t="s">
         <v>4</v>
@@ -19730,10 +19706,10 @@
         <v>988</v>
       </c>
       <c r="E877" s="2" t="s">
-        <v>1848</v>
+        <v>1841</v>
       </c>
       <c r="F877" s="2" t="s">
-        <v>1859</v>
+        <v>1852</v>
       </c>
     </row>
     <row r="878" spans="1:12" x14ac:dyDescent="0.25">
@@ -19988,7 +19964,7 @@
         <v>988</v>
       </c>
       <c r="E895" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="896" spans="1:5" x14ac:dyDescent="0.25">
@@ -20117,7 +20093,7 @@
         <v>988</v>
       </c>
       <c r="E904" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="905" spans="1:5" x14ac:dyDescent="0.25">
@@ -20302,7 +20278,7 @@
         <v>988</v>
       </c>
       <c r="E917" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="918" spans="1:5" x14ac:dyDescent="0.25">
@@ -20683,7 +20659,7 @@
         <v>988</v>
       </c>
       <c r="E944" s="2" t="s">
-        <v>1927</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="945" spans="1:5" x14ac:dyDescent="0.25">
@@ -20728,7 +20704,7 @@
         <v>988</v>
       </c>
       <c r="E947" s="2" t="s">
-        <v>1935</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="948" spans="1:5" x14ac:dyDescent="0.25">
@@ -20745,7 +20721,7 @@
         <v>988</v>
       </c>
       <c r="E948" s="2" t="s">
-        <v>1927</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="949" spans="1:5" x14ac:dyDescent="0.25">
@@ -20762,7 +20738,7 @@
         <v>988</v>
       </c>
       <c r="E949" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="950" spans="1:5" x14ac:dyDescent="0.25">
@@ -20975,7 +20951,7 @@
         <v>988</v>
       </c>
       <c r="E964" s="4" t="s">
-        <v>1929</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="965" spans="1:5" x14ac:dyDescent="0.25">
@@ -21090,7 +21066,7 @@
         <v>988</v>
       </c>
       <c r="E972" s="2" t="s">
-        <v>1850</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="973" spans="1:5" x14ac:dyDescent="0.25">
@@ -21373,7 +21349,7 @@
         <v>988</v>
       </c>
       <c r="E992" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="993" spans="1:11" x14ac:dyDescent="0.25">
@@ -21421,13 +21397,13 @@
         <v>277</v>
       </c>
       <c r="F995" s="2" t="s">
-        <v>1859</v>
+        <v>1852</v>
       </c>
       <c r="G995" s="2">
         <v>41</v>
       </c>
       <c r="K995" s="7" t="s">
-        <v>1791</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="996" spans="1:11" x14ac:dyDescent="0.25">
@@ -21444,7 +21420,7 @@
         <v>988</v>
       </c>
       <c r="E996" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="997" spans="1:11" x14ac:dyDescent="0.25">
@@ -21573,16 +21549,16 @@
         <v>988</v>
       </c>
       <c r="E1005" s="2" t="s">
-        <v>1862</v>
+        <v>1855</v>
       </c>
       <c r="F1005" s="2" t="s">
-        <v>1849</v>
+        <v>1842</v>
       </c>
       <c r="G1005" s="2">
         <v>42</v>
       </c>
       <c r="K1005" s="7" t="s">
-        <v>1802</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="1006" spans="1:11" x14ac:dyDescent="0.25">
@@ -21725,7 +21701,7 @@
         <v>988</v>
       </c>
       <c r="E1015" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1016" spans="1:5" x14ac:dyDescent="0.25">
@@ -21980,7 +21956,7 @@
         <v>988</v>
       </c>
       <c r="E1033" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1034" spans="1:11" x14ac:dyDescent="0.25">
@@ -21997,7 +21973,7 @@
         <v>988</v>
       </c>
       <c r="E1034" s="2" t="s">
-        <v>1888</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="1035" spans="1:11" x14ac:dyDescent="0.25">
@@ -22056,13 +22032,13 @@
         <v>988</v>
       </c>
       <c r="E1038" s="2" t="s">
-        <v>1880</v>
+        <v>1873</v>
       </c>
       <c r="H1038" s="2">
         <v>50</v>
       </c>
       <c r="K1038" s="7" t="s">
-        <v>1848</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="1039" spans="1:11" x14ac:dyDescent="0.25">
@@ -22093,7 +22069,7 @@
         <v>988</v>
       </c>
       <c r="E1040" s="2" t="s">
-        <v>1888</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="1041" spans="1:5" x14ac:dyDescent="0.25">
@@ -22124,7 +22100,7 @@
         <v>988</v>
       </c>
       <c r="E1042" s="2" t="s">
-        <v>1910</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="1043" spans="1:5" x14ac:dyDescent="0.25">
@@ -22183,7 +22159,7 @@
         <v>988</v>
       </c>
       <c r="E1046" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1047" spans="1:5" x14ac:dyDescent="0.25">
@@ -22480,13 +22456,13 @@
         <v>988</v>
       </c>
       <c r="E1067" s="2" t="s">
-        <v>1850</v>
+        <v>1843</v>
       </c>
       <c r="F1067" s="2" t="s">
-        <v>1859</v>
+        <v>1852</v>
       </c>
       <c r="K1067" s="7" t="s">
-        <v>1850</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="1068" spans="1:11" x14ac:dyDescent="0.25">
@@ -22573,7 +22549,7 @@
         <v>988</v>
       </c>
       <c r="E1073" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1074" spans="1:7" x14ac:dyDescent="0.25">
@@ -22590,10 +22566,10 @@
         <v>988</v>
       </c>
       <c r="E1074" s="2" t="s">
-        <v>1889</v>
+        <v>1882</v>
       </c>
       <c r="F1074" s="2" t="s">
-        <v>1857</v>
+        <v>1850</v>
       </c>
       <c r="G1074" s="2">
         <v>180</v>
@@ -22837,16 +22813,16 @@
         <v>988</v>
       </c>
       <c r="E1091" s="4" t="s">
-        <v>1908</v>
+        <v>1901</v>
       </c>
       <c r="F1091" s="2" t="s">
-        <v>1853</v>
+        <v>1846</v>
       </c>
       <c r="H1091" s="2">
         <v>55</v>
       </c>
       <c r="K1091" s="7" t="s">
-        <v>1851</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="1092" spans="1:11" x14ac:dyDescent="0.25">
@@ -22947,7 +22923,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="1099" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1099" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A1099" s="3">
         <v>3293</v>
       </c>
@@ -22961,10 +22937,10 @@
         <v>988</v>
       </c>
       <c r="E1099" s="4" t="s">
-        <v>1909</v>
+        <v>1902</v>
       </c>
       <c r="F1099" s="2" t="s">
-        <v>1857</v>
+        <v>1850</v>
       </c>
       <c r="G1099" s="2">
         <v>700</v>
@@ -22976,7 +22952,7 @@
         <v>1080</v>
       </c>
       <c r="K1099" s="7" t="s">
-        <v>1792</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="1100" spans="1:11" x14ac:dyDescent="0.25">
@@ -23119,16 +23095,16 @@
         <v>988</v>
       </c>
       <c r="E1109" s="2" t="s">
-        <v>1786</v>
+        <v>1780</v>
       </c>
       <c r="F1109" s="2" t="s">
-        <v>1859</v>
+        <v>1852</v>
       </c>
       <c r="G1109" s="2">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="K1109" s="7" t="s">
-        <v>1786</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="1110" spans="1:11" x14ac:dyDescent="0.25">
@@ -23201,7 +23177,7 @@
         <v>988</v>
       </c>
       <c r="E1114" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1115" spans="1:11" x14ac:dyDescent="0.25">
@@ -23218,7 +23194,7 @@
         <v>988</v>
       </c>
       <c r="E1115" s="2" t="s">
-        <v>1949</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="1116" spans="1:11" x14ac:dyDescent="0.25">
@@ -23437,7 +23413,7 @@
         <v>988</v>
       </c>
       <c r="E1130" s="2" t="s">
-        <v>1879</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="1131" spans="1:11" x14ac:dyDescent="0.25">
@@ -23482,16 +23458,16 @@
         <v>988</v>
       </c>
       <c r="E1133" s="2" t="s">
-        <v>1786</v>
+        <v>1780</v>
       </c>
       <c r="F1133" s="2" t="s">
-        <v>1859</v>
+        <v>1852</v>
       </c>
       <c r="G1133" s="2">
         <v>65</v>
       </c>
       <c r="K1133" s="7" t="s">
-        <v>1786</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="1134" spans="1:11" x14ac:dyDescent="0.25">
@@ -23718,7 +23694,7 @@
         <v>988</v>
       </c>
       <c r="E1149" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1150" spans="1:5" x14ac:dyDescent="0.25">
@@ -23791,7 +23767,7 @@
         <v>988</v>
       </c>
       <c r="E1154" s="2" t="s">
-        <v>1848</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="1155" spans="1:11" x14ac:dyDescent="0.25">
@@ -23822,7 +23798,7 @@
         <v>988</v>
       </c>
       <c r="E1156" s="4" t="s">
-        <v>1911</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="1157" spans="1:11" x14ac:dyDescent="0.25">
@@ -23853,7 +23829,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="1159" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="1159" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A1159" s="3">
         <v>3552</v>
       </c>
@@ -23867,10 +23843,10 @@
         <v>988</v>
       </c>
       <c r="E1159" s="4" t="s">
-        <v>1915</v>
+        <v>1948</v>
       </c>
       <c r="F1159" s="2" t="s">
-        <v>1857</v>
+        <v>1850</v>
       </c>
       <c r="G1159" s="2">
         <v>140</v>
@@ -23879,7 +23855,7 @@
         <v>183</v>
       </c>
       <c r="K1159" s="7" t="s">
-        <v>1781</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="1160" spans="1:11" x14ac:dyDescent="0.25">
@@ -24176,7 +24152,7 @@
         <v>988</v>
       </c>
       <c r="E1180" s="2" t="s">
-        <v>1949</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="1181" spans="1:5" x14ac:dyDescent="0.25">
@@ -24409,7 +24385,7 @@
         <v>988</v>
       </c>
       <c r="E1196" s="2" t="s">
-        <v>1783</v>
+        <v>1777</v>
       </c>
       <c r="G1196" s="2">
         <v>160</v>
@@ -24639,16 +24615,16 @@
         <v>988</v>
       </c>
       <c r="E1212" s="4" t="s">
-        <v>1869</v>
+        <v>1862</v>
       </c>
       <c r="F1212" s="2" t="s">
-        <v>1849</v>
+        <v>1842</v>
       </c>
       <c r="G1212" s="2">
         <v>61</v>
       </c>
       <c r="K1212" s="7" t="s">
-        <v>1802</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="1213" spans="1:11" x14ac:dyDescent="0.25">
@@ -24987,7 +24963,7 @@
         <v>988</v>
       </c>
       <c r="E1236" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1237" spans="1:5" x14ac:dyDescent="0.25">
@@ -26096,16 +26072,16 @@
         <v>988</v>
       </c>
       <c r="E1315" s="4" t="s">
-        <v>1886</v>
+        <v>1879</v>
       </c>
       <c r="F1315" s="2" t="s">
-        <v>1849</v>
+        <v>1842</v>
       </c>
       <c r="G1315" s="2">
         <v>30</v>
       </c>
       <c r="K1315" s="7" t="s">
-        <v>1887</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="1316" spans="1:11" x14ac:dyDescent="0.25">
@@ -26164,7 +26140,7 @@
         <v>988</v>
       </c>
       <c r="E1319" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1320" spans="1:11" x14ac:dyDescent="0.25">
@@ -26181,7 +26157,7 @@
         <v>988</v>
       </c>
       <c r="E1320" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1321" spans="1:11" x14ac:dyDescent="0.25">
@@ -26450,7 +26426,7 @@
         <v>988</v>
       </c>
       <c r="E1339" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1340" spans="1:5" x14ac:dyDescent="0.25">
@@ -26467,7 +26443,7 @@
         <v>988</v>
       </c>
       <c r="E1340" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1341" spans="1:5" x14ac:dyDescent="0.25">
@@ -26652,7 +26628,7 @@
         <v>988</v>
       </c>
       <c r="E1353" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1354" spans="1:5" x14ac:dyDescent="0.25">
@@ -26809,7 +26785,7 @@
         <v>988</v>
       </c>
       <c r="E1364" s="2" t="s">
-        <v>1927</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="1365" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -26826,10 +26802,10 @@
         <v>988</v>
       </c>
       <c r="E1365" s="4" t="s">
-        <v>1940</v>
+        <v>1932</v>
       </c>
       <c r="F1365" s="2" t="s">
-        <v>1859</v>
+        <v>1852</v>
       </c>
       <c r="G1365" s="2">
         <v>40</v>
@@ -26838,10 +26814,10 @@
         <v>48.2</v>
       </c>
       <c r="K1365" s="7" t="s">
+        <v>1784</v>
+      </c>
+      <c r="L1365" s="5" t="s">
         <v>1790</v>
-      </c>
-      <c r="L1365" s="5" t="s">
-        <v>1797</v>
       </c>
     </row>
     <row r="1366" spans="1:12" x14ac:dyDescent="0.25">
@@ -26998,7 +26974,7 @@
         <v>988</v>
       </c>
       <c r="E1376" s="4" t="s">
-        <v>1917</v>
+        <v>1909</v>
       </c>
       <c r="G1376" s="2">
         <v>85</v>
@@ -27256,13 +27232,13 @@
         <v>988</v>
       </c>
       <c r="E1394" s="4" t="s">
-        <v>1884</v>
+        <v>1877</v>
       </c>
       <c r="G1394" s="2">
         <v>65</v>
       </c>
       <c r="L1394" s="5" t="s">
-        <v>1885</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="1395" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
@@ -27279,7 +27255,7 @@
         <v>988</v>
       </c>
       <c r="E1395" s="4" t="s">
-        <v>1919</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="1396" spans="1:12" x14ac:dyDescent="0.25">
@@ -27310,7 +27286,7 @@
         <v>988</v>
       </c>
       <c r="E1397" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1398" spans="1:12" x14ac:dyDescent="0.25">
@@ -27341,7 +27317,7 @@
         <v>988</v>
       </c>
       <c r="E1399" s="2" t="s">
-        <v>1897</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="1400" spans="1:12" x14ac:dyDescent="0.25">
@@ -27414,7 +27390,7 @@
         <v>988</v>
       </c>
       <c r="E1404" s="2" t="s">
-        <v>1848</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="1405" spans="1:12" x14ac:dyDescent="0.25">
@@ -27445,7 +27421,7 @@
         <v>988</v>
       </c>
       <c r="E1406" s="2" t="s">
-        <v>1910</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="1407" spans="1:12" x14ac:dyDescent="0.25">
@@ -27476,7 +27452,7 @@
         <v>988</v>
       </c>
       <c r="E1408" s="4" t="s">
-        <v>1916</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="1409" spans="1:5" x14ac:dyDescent="0.25">
@@ -27563,7 +27539,7 @@
         <v>988</v>
       </c>
       <c r="E1414" s="2" t="s">
-        <v>1913</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="1415" spans="1:5" x14ac:dyDescent="0.25">
@@ -27776,7 +27752,7 @@
         <v>988</v>
       </c>
       <c r="E1429" s="2" t="s">
-        <v>1862</v>
+        <v>1855</v>
       </c>
       <c r="G1429" s="2">
         <v>60</v>
@@ -27894,7 +27870,7 @@
         <v>988</v>
       </c>
       <c r="E1437" s="2" t="s">
-        <v>1937</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="1438" spans="1:7" x14ac:dyDescent="0.25">
@@ -27911,7 +27887,7 @@
         <v>988</v>
       </c>
       <c r="E1438" s="2" t="s">
-        <v>1890</v>
+        <v>1883</v>
       </c>
       <c r="G1438" s="2">
         <v>430</v>
@@ -28048,7 +28024,7 @@
         <v>6104</v>
       </c>
       <c r="B1448" s="1" t="s">
-        <v>1891</v>
+        <v>1884</v>
       </c>
       <c r="C1448" s="2" t="s">
         <v>1763</v>
@@ -28057,7 +28033,7 @@
         <v>988</v>
       </c>
       <c r="E1448" s="2" t="s">
-        <v>1892</v>
+        <v>1885</v>
       </c>
       <c r="K1448" s="7" t="s">
         <v>1767</v>
@@ -28234,7 +28210,7 @@
         <v>988</v>
       </c>
       <c r="E1460" s="2" t="s">
-        <v>1863</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="1461" spans="1:5" x14ac:dyDescent="0.25">
@@ -28293,7 +28269,7 @@
         <v>988</v>
       </c>
       <c r="E1464" s="4" t="s">
-        <v>1926</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="1465" spans="1:5" x14ac:dyDescent="0.25">
@@ -28520,7 +28496,7 @@
         <v>988</v>
       </c>
       <c r="E1480" s="2" t="s">
-        <v>1910</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="1481" spans="1:5" x14ac:dyDescent="0.25">
@@ -28565,7 +28541,7 @@
         <v>988</v>
       </c>
       <c r="E1483" s="4" t="s">
-        <v>1921</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="1484" spans="1:5" x14ac:dyDescent="0.25">
@@ -28624,7 +28600,7 @@
         <v>988</v>
       </c>
       <c r="E1487" s="2" t="s">
-        <v>1888</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="1488" spans="1:5" x14ac:dyDescent="0.25">
@@ -28641,7 +28617,7 @@
         <v>988</v>
       </c>
       <c r="E1488" s="2" t="s">
-        <v>1925</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="1489" spans="1:12" x14ac:dyDescent="0.25">
@@ -28689,16 +28665,16 @@
         <v>277</v>
       </c>
       <c r="F1491" s="2" t="s">
-        <v>1857</v>
+        <v>1850</v>
       </c>
       <c r="G1491" s="2">
         <v>80</v>
       </c>
       <c r="K1491" s="7" t="s">
-        <v>1791</v>
+        <v>1785</v>
       </c>
       <c r="L1491" s="5" t="s">
-        <v>1789</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="1492" spans="1:12" x14ac:dyDescent="0.25">
@@ -28813,7 +28789,7 @@
         <v>988</v>
       </c>
       <c r="E1499" s="4" t="s">
-        <v>1896</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="1500" spans="1:12" x14ac:dyDescent="0.25">
@@ -28956,7 +28932,7 @@
         <v>988</v>
       </c>
       <c r="E1509" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1510" spans="1:12" x14ac:dyDescent="0.25">
@@ -28987,10 +28963,10 @@
         <v>988</v>
       </c>
       <c r="E1511" s="4" t="s">
-        <v>1941</v>
+        <v>1933</v>
       </c>
       <c r="F1511" s="2" t="s">
-        <v>1859</v>
+        <v>1852</v>
       </c>
       <c r="G1511" s="2">
         <v>100</v>
@@ -29052,7 +29028,7 @@
         <v>988</v>
       </c>
       <c r="E1515" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1516" spans="1:12" x14ac:dyDescent="0.25">
@@ -29069,7 +29045,7 @@
         <v>988</v>
       </c>
       <c r="E1516" s="4" t="s">
-        <v>1848</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="1517" spans="1:12" x14ac:dyDescent="0.25">
@@ -29105,7 +29081,7 @@
         <v>6237</v>
       </c>
       <c r="B1519" s="1" t="s">
-        <v>1811</v>
+        <v>1804</v>
       </c>
       <c r="C1519" s="2" t="s">
         <v>1763</v>
@@ -29114,13 +29090,13 @@
         <v>988</v>
       </c>
       <c r="E1519" s="4" t="s">
+        <v>1841</v>
+      </c>
+      <c r="F1519" s="2" t="s">
         <v>1848</v>
       </c>
-      <c r="F1519" s="2" t="s">
-        <v>1855</v>
-      </c>
       <c r="L1519" s="5" t="s">
-        <v>1810</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="1520" spans="1:12" x14ac:dyDescent="0.25">
@@ -29389,7 +29365,7 @@
         <v>988</v>
       </c>
       <c r="E1538" s="4" t="s">
-        <v>1921</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="1539" spans="1:5" x14ac:dyDescent="0.25">
@@ -29560,7 +29536,7 @@
         <v>988</v>
       </c>
       <c r="E1550" s="2" t="s">
-        <v>1897</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="1551" spans="1:5" x14ac:dyDescent="0.25">
@@ -29619,16 +29595,16 @@
         <v>988</v>
       </c>
       <c r="E1554" s="4" t="s">
-        <v>1874</v>
+        <v>1867</v>
       </c>
       <c r="F1554" s="2" t="s">
-        <v>1857</v>
+        <v>1850</v>
       </c>
       <c r="G1554" s="2">
         <v>130</v>
       </c>
       <c r="K1554" s="7" t="s">
-        <v>1782</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="1555" spans="1:11" x14ac:dyDescent="0.25">
@@ -29799,7 +29775,7 @@
         <v>988</v>
       </c>
       <c r="E1566" s="2" t="s">
-        <v>1925</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="1567" spans="1:11" x14ac:dyDescent="0.25">
@@ -29900,7 +29876,7 @@
         <v>988</v>
       </c>
       <c r="E1573" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1574" spans="1:11" x14ac:dyDescent="0.25">
@@ -30043,16 +30019,16 @@
         <v>988</v>
       </c>
       <c r="E1583" s="2" t="s">
-        <v>1783</v>
+        <v>1777</v>
       </c>
       <c r="F1583" s="2" t="s">
-        <v>1855</v>
+        <v>1848</v>
       </c>
       <c r="H1583" s="2">
         <v>220</v>
       </c>
       <c r="K1583" s="7" t="s">
-        <v>1783</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="1584" spans="1:11" x14ac:dyDescent="0.25">
@@ -30060,7 +30036,7 @@
         <v>6542</v>
       </c>
       <c r="B1584" s="1" t="s">
-        <v>1893</v>
+        <v>1886</v>
       </c>
       <c r="C1584" s="2" t="s">
         <v>1763</v>
@@ -30069,7 +30045,7 @@
         <v>988</v>
       </c>
       <c r="E1584" s="2" t="s">
-        <v>1888</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="1585" spans="1:5" x14ac:dyDescent="0.25">
@@ -30282,7 +30258,7 @@
         <v>988</v>
       </c>
       <c r="E1599" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1600" spans="1:5" x14ac:dyDescent="0.25">
@@ -30565,7 +30541,7 @@
         <v>988</v>
       </c>
       <c r="E1619" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1620" spans="1:7" x14ac:dyDescent="0.25">
@@ -30596,7 +30572,7 @@
         <v>988</v>
       </c>
       <c r="E1621" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1622" spans="1:7" x14ac:dyDescent="0.25">
@@ -30711,7 +30687,7 @@
         <v>988</v>
       </c>
       <c r="E1629" s="4" t="s">
-        <v>1919</v>
+        <v>1911</v>
       </c>
       <c r="G1629" s="2">
         <v>70</v>
@@ -31053,7 +31029,7 @@
         <v>988</v>
       </c>
       <c r="E1653" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1654" spans="1:7" x14ac:dyDescent="0.25">
@@ -31098,7 +31074,7 @@
         <v>988</v>
       </c>
       <c r="E1656" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1657" spans="1:7" x14ac:dyDescent="0.25">
@@ -31129,10 +31105,10 @@
         <v>988</v>
       </c>
       <c r="E1658" s="4" t="s">
-        <v>1876</v>
+        <v>1869</v>
       </c>
       <c r="F1658" s="2" t="s">
-        <v>1849</v>
+        <v>1842</v>
       </c>
       <c r="G1658" s="2">
         <v>26</v>
@@ -31586,7 +31562,7 @@
         <v>988</v>
       </c>
       <c r="E1690" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1691" spans="1:5" x14ac:dyDescent="0.25">
@@ -32177,7 +32153,7 @@
         <v>988</v>
       </c>
       <c r="E1732" s="2" t="s">
-        <v>1894</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="1733" spans="1:5" x14ac:dyDescent="0.25">
@@ -32390,10 +32366,10 @@
         <v>988</v>
       </c>
       <c r="E1747" s="4" t="s">
-        <v>1950</v>
+        <v>1942</v>
       </c>
       <c r="F1747" s="2" t="s">
-        <v>1849</v>
+        <v>1842</v>
       </c>
       <c r="G1747" s="2">
         <v>40</v>
@@ -32427,168 +32403,168 @@
   <sheetData>
     <row r="2" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>1839</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
-        <v>1813</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>1814</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
-        <v>1815</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>1816</v>
+        <v>1809</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>1817</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
-        <v>1818</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>1819</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
-        <v>1820</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="11" t="s">
-        <v>1821</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>1824</v>
+        <v>1817</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1822</v>
+        <v>1815</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="11" t="s">
-        <v>1823</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16" s="12" t="s">
-        <v>1825</v>
+        <v>1818</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>1826</v>
+        <v>1819</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>1827</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="15"/>
       <c r="D17" s="16"/>
       <c r="E17" s="17" t="s">
-        <v>1828</v>
+        <v>1821</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" s="15"/>
       <c r="D18" s="16"/>
       <c r="E18" s="17" t="s">
-        <v>1829</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="15"/>
       <c r="D19" s="16"/>
       <c r="E19" s="17" t="s">
-        <v>1830</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="20" spans="3:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="18"/>
       <c r="D20" s="19"/>
       <c r="E20" s="20" t="s">
-        <v>1831</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="21" spans="3:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" s="12" t="s">
-        <v>1832</v>
+        <v>1825</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>1838</v>
+        <v>1831</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>1833</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C23" s="15"/>
       <c r="D23" s="16"/>
       <c r="E23" s="17" t="s">
-        <v>1832</v>
+        <v>1825</v>
       </c>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C24" s="15"/>
       <c r="D24" s="16"/>
       <c r="E24" s="17" t="s">
-        <v>1834</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C25" s="15"/>
       <c r="D25" s="16"/>
       <c r="E25" s="17" t="s">
-        <v>1835</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C26" s="15"/>
       <c r="D26" s="16"/>
       <c r="E26" s="17" t="s">
-        <v>1836</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="27" spans="3:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="18"/>
       <c r="D27" s="19"/>
       <c r="E27" s="20" t="s">
-        <v>1837</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="28" spans="3:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C29" s="12" t="s">
+        <v>1833</v>
+      </c>
+      <c r="D29" s="13" t="s">
         <v>1840</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>1847</v>
       </c>
       <c r="E29" s="22">
         <v>44151</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>1841</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.25">
@@ -32596,7 +32572,7 @@
       <c r="D30" s="16"/>
       <c r="E30" s="16"/>
       <c r="F30" s="17" t="s">
-        <v>1842</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.25">
@@ -32604,7 +32580,7 @@
       <c r="D31" s="16"/>
       <c r="E31" s="16"/>
       <c r="F31" s="17" t="s">
-        <v>1843</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.25">
@@ -32612,7 +32588,7 @@
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
       <c r="F32" s="17" t="s">
-        <v>1844</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
@@ -32620,7 +32596,7 @@
       <c r="D33" s="16"/>
       <c r="E33" s="16"/>
       <c r="F33" s="17" t="s">
-        <v>1845</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="34" spans="3:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -32628,7 +32604,7 @@
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
       <c r="F34" s="20" t="s">
-        <v>1846</v>
+        <v>1839</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update hold stock and hold price
</commit_message>
<xml_diff>
--- a/all_stock.xlsx
+++ b/all_stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\download\rich_stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06701EC4-E66B-4C7D-AC42-770820C9287F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D45683-ED7B-4E7F-BE82-4872C47155B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7249,8 +7249,8 @@
   <dimension ref="A1:N1713"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1084" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1093" sqref="I1093"/>
+      <pane ySplit="1" topLeftCell="A277" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I288" sqref="I288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -11626,6 +11626,9 @@
       <c r="E287" s="2" t="s">
         <v>1763</v>
       </c>
+      <c r="I287" s="2">
+        <v>27.5</v>
+      </c>
     </row>
     <row r="288" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A288" s="3">
@@ -15056,10 +15059,7 @@
         <v>1833</v>
       </c>
       <c r="G509" s="2">
-        <v>60</v>
-      </c>
-      <c r="I509" s="2">
-        <v>64.5</v>
+        <v>71</v>
       </c>
       <c r="M509" s="7"/>
     </row>
@@ -23721,9 +23721,6 @@
       <c r="G1072" s="2">
         <v>800</v>
       </c>
-      <c r="I1072" s="2">
-        <v>808</v>
-      </c>
       <c r="M1072" s="7" t="s">
         <v>1835</v>
       </c>
@@ -23976,7 +23973,7 @@
         <v>1830</v>
       </c>
     </row>
-    <row r="1089" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1089" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1089" s="3">
         <v>3363</v>
       </c>
@@ -23990,7 +23987,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="1090" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1090" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1090" s="3">
         <v>3372</v>
       </c>
@@ -24004,7 +24001,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="1091" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1091" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1091" s="3">
         <v>3373</v>
       </c>
@@ -24018,7 +24015,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="1092" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1092" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1092" s="3">
         <v>3374</v>
       </c>
@@ -24037,11 +24034,8 @@
       <c r="G1092" s="2">
         <v>180</v>
       </c>
-      <c r="I1092" s="2">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="1093" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1093" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1093" s="3">
         <v>3379</v>
       </c>
@@ -24055,7 +24049,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="1094" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1094" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1094" s="3">
         <v>3388</v>
       </c>
@@ -24069,7 +24063,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="1095" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1095" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1095" s="3">
         <v>3390</v>
       </c>
@@ -24083,7 +24077,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="1096" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1096" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1096" s="3">
         <v>3402</v>
       </c>
@@ -24097,7 +24091,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="1097" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1097" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1097" s="3">
         <v>3426</v>
       </c>
@@ -24111,7 +24105,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="1098" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1098" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1098" s="3">
         <v>3434</v>
       </c>
@@ -24125,7 +24119,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="1099" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1099" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1099" s="3">
         <v>3438</v>
       </c>
@@ -24139,7 +24133,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="1100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1100" s="3">
         <v>3441</v>
       </c>
@@ -24153,7 +24147,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="1101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1101" s="3">
         <v>3444</v>
       </c>
@@ -24167,7 +24161,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="1102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1102" s="3">
         <v>3455</v>
       </c>
@@ -24181,7 +24175,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="1103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1103" s="3">
         <v>3465</v>
       </c>
@@ -24198,7 +24192,7 @@
         <v>1780</v>
       </c>
     </row>
-    <row r="1104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1104" s="3">
         <v>3466</v>
       </c>

</xml_diff>

<commit_message>
update new info file
</commit_message>
<xml_diff>
--- a/all_stock.xlsx
+++ b/all_stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\download\rich_stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0ADBDD4-5CE3-46D5-B7C6-322FCE93EC49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287ECBBF-631B-42F2-A544-171FA55C3DCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7249,8 +7249,8 @@
   <dimension ref="A1:N1713"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I276" sqref="I276"/>
+      <pane ySplit="1" topLeftCell="A1074" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1083" sqref="I1083"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -11623,9 +11623,6 @@
       <c r="E287" s="2" t="s">
         <v>1763</v>
       </c>
-      <c r="I287" s="2">
-        <v>27.5</v>
-      </c>
     </row>
     <row r="288" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A288" s="3">
@@ -11686,7 +11683,7 @@
         <v>1763</v>
       </c>
       <c r="I291" s="2">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="292" spans="1:9" x14ac:dyDescent="0.3">
@@ -12171,9 +12168,6 @@
       <c r="E321" s="2" t="s">
         <v>1868</v>
       </c>
-      <c r="I321" s="2">
-        <v>26.05</v>
-      </c>
     </row>
     <row r="322" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A322" s="3">
@@ -23873,8 +23867,8 @@
       <c r="F1082" s="2" t="s">
         <v>1917</v>
       </c>
-      <c r="G1082" s="2">
-        <v>200</v>
+      <c r="I1082" s="2">
+        <v>226</v>
       </c>
     </row>
     <row r="1083" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
[update] 6 and 7 information
</commit_message>
<xml_diff>
--- a/all_stock.xlsx
+++ b/all_stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\download\rich_stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92725372-1774-4126-82D6-60687476DA74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A818ECF-C8C0-4302-8E29-E0579FAFC7BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5893" uniqueCount="2181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5909" uniqueCount="2189">
   <si>
     <t>代碼</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -5731,11 +5731,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>等到營收要起來才行
-目標營收 3E</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>電機機械</t>
   </si>
   <si>
@@ -6041,11 +6036,6 @@
   </si>
   <si>
     <t>連接器</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>伺服器，其次是筆電產品和車用產品
-凡甲主業為伺服器用線</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -6132,10 +6122,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>自動化系統</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>設備廠</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6218,13 +6204,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>9月 EPS 0.9
-10月 EPS 1.08
-11月營收新高
-2021 EPS上看15 ~ 18塊</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>磊晶矽晶圓</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6322,10 +6301,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>短期注意</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>全球第2大PPTC廠
 營收占比 77%
 合併德商，衝全球第一大散熱基板廠
@@ -6357,10 +6332,6 @@
   </si>
   <si>
     <t>鞋材</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>配息率太低</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -6493,10 +6464,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2020估 4塊，配息3塊。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>半導體</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6506,10 +6473,6 @@
   </si>
   <si>
     <t>運動</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>衛星</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -6865,10 +6828,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>太陽能股中營收比較好，也有在擴廠。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>衛星</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6888,10 +6847,6 @@
   </si>
   <si>
     <t>[2020 EPS] 11.57</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>衛星</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -7001,10 +6956,6 @@
   </si>
   <si>
     <t>[2020 EPS] 4.31</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[2020 EPS] 11.3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -7066,10 +7017,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[2020 EPS] 4.04</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[2020 EPS] 2.04</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7247,11 +7194,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[2020 EPS] 6.31
-泰鼎四大產品線包括HOME、通訊、PC、車用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>4.56</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7261,7 +7203,106 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>短期注意</t>
+    <t>晶技1月稅前EPS為0.85元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>太陽能股中營收比較好，也有在擴廠。
+不配股配息。不投資。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不投資</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>配息率太低
+百和1月EPS0.57元
+[2020 EPS] 5.24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9月 EPS 0.9
+10月 EPS 1.08
+同致1月獲利年增78倍 每股賺1.18元</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>核心</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[2020 EPS] 3.59</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自動化系統
+2021/01 營收大減。
+2020 EPS太少，2021 配息不高。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[2020 EPS] -1.24
+營收要上3E 才有看頭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>定存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[2020 EPS] 4.04
+不賣的定存股</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IPC(工業電腦)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[2020 EPS] 6.07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[2020 EPS] 6.31
+泰鼎四大產品線包括HOME、通訊、PC、車用
+營收成長中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>被動元件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[2020 EPS] 11.3
+銅箔基板(CCL)52.80%
+《電子零件》HDI板夯 台光電今年營運攀峰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>伺服器，其次是筆電產品和車用產品
+凡甲主業為伺服器用線
+[2020 EPS] 7.25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9.58</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7815,9 +7856,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1713"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1052" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1060" sqref="G1060"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1114" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1123" sqref="K1123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -7855,7 +7896,7 @@
         <v>1821</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>1919</v>
+        <v>1917</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>1721</v>
@@ -7870,16 +7911,16 @@
         <v>1715</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>2123</v>
+        <v>2113</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>1990</v>
+        <v>1984</v>
       </c>
       <c r="M1" s="5" t="s">
         <v>1702</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>1998</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.3">
@@ -7896,10 +7937,10 @@
         <v>941</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>1882</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>1883</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>1884</v>
       </c>
       <c r="G2" s="2">
         <v>40.5</v>
@@ -8118,7 +8159,7 @@
         <v>941</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="K16" s="27"/>
     </row>
@@ -8151,7 +8192,7 @@
         <v>941</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>1767</v>
@@ -8235,7 +8276,7 @@
         <v>941</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>1767</v>
@@ -8334,11 +8375,11 @@
         <v>941</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>2050</v>
+        <v>2042</v>
       </c>
       <c r="K29" s="27"/>
       <c r="M29" s="5" t="s">
-        <v>2054</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -8569,7 +8610,7 @@
       </c>
       <c r="K44" s="27"/>
       <c r="M44" s="5" t="s">
-        <v>2117</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
@@ -8619,11 +8660,11 @@
         <v>941</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>2050</v>
+        <v>2042</v>
       </c>
       <c r="K47" s="27"/>
       <c r="M47" s="5" t="s">
-        <v>2051</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
@@ -8775,11 +8816,11 @@
         <v>1813</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>2154</v>
+        <v>2142</v>
       </c>
       <c r="K56" s="27"/>
       <c r="M56" s="5" t="s">
-        <v>2155</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
@@ -9462,17 +9503,17 @@
         <v>941</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>2156</v>
+        <v>2144</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>2157</v>
+        <v>2145</v>
       </c>
       <c r="G101" s="2">
         <v>150</v>
       </c>
       <c r="K101" s="27"/>
       <c r="M101" s="5" t="s">
-        <v>2158</v>
+        <v>2146</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.3">
@@ -9543,7 +9584,7 @@
         <v>1825</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>2118</v>
+        <v>2108</v>
       </c>
       <c r="G105" s="2">
         <v>51.5</v>
@@ -9585,7 +9626,7 @@
         <v>1825</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="G107" s="2">
         <v>47</v>
@@ -9593,7 +9634,7 @@
       <c r="K107" s="27"/>
       <c r="L107" s="4"/>
       <c r="M107" s="5" t="s">
-        <v>1946</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.3">
@@ -9614,7 +9655,7 @@
       </c>
       <c r="K108" s="27"/>
       <c r="M108" s="5" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.3">
@@ -9667,14 +9708,14 @@
         <v>1808</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="G111" s="2">
-        <v>13</v>
+        <v>13.5</v>
       </c>
       <c r="K111" s="27"/>
       <c r="M111" s="5" t="s">
-        <v>2086</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.3">
@@ -10045,10 +10086,10 @@
         <v>941</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>1966</v>
+        <v>1962</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>1968</v>
+        <v>1964</v>
       </c>
       <c r="K135" s="27"/>
     </row>
@@ -10099,11 +10140,11 @@
         <v>1759</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="K138" s="27"/>
       <c r="M138" s="5" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.3">
@@ -10121,7 +10162,7 @@
       </c>
       <c r="K139" s="27"/>
       <c r="M139" s="5" t="s">
-        <v>2072</v>
+        <v>2064</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.3">
@@ -10210,13 +10251,19 @@
         <v>941</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>2037</v>
+        <v>2029</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>2178</v>
+      </c>
+      <c r="G144" s="2">
+        <v>15</v>
       </c>
       <c r="K144" s="27">
         <v>0.9</v>
       </c>
       <c r="M144" s="5" t="s">
-        <v>2135</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.3">
@@ -10255,7 +10302,7 @@
       </c>
       <c r="K146" s="27"/>
       <c r="M146" s="5" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.3">
@@ -10408,7 +10455,7 @@
       </c>
       <c r="K156" s="27"/>
       <c r="M156" s="5" t="s">
-        <v>2070</v>
+        <v>2062</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.3">
@@ -10575,11 +10622,11 @@
         <v>941</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="K167" s="27"/>
       <c r="M167" s="5" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.3">
@@ -10761,7 +10808,7 @@
         <v>941</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="K179" s="27"/>
     </row>
@@ -10797,11 +10844,11 @@
         <v>1770</v>
       </c>
       <c r="F181" s="2" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="K181" s="27"/>
       <c r="M181" s="5" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.3">
@@ -10833,7 +10880,7 @@
         <v>941</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="K183" s="27"/>
     </row>
@@ -11091,19 +11138,19 @@
         <v>941</v>
       </c>
       <c r="E200" s="2" t="s">
-        <v>2160</v>
+        <v>2148</v>
       </c>
       <c r="F200" s="2" t="s">
-        <v>2161</v>
+        <v>2149</v>
       </c>
       <c r="G200" s="2">
         <v>11</v>
       </c>
       <c r="K200" s="27" t="s">
-        <v>2159</v>
+        <v>2147</v>
       </c>
       <c r="M200" s="5" t="s">
-        <v>2162</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="201" spans="1:13" x14ac:dyDescent="0.3">
@@ -11288,7 +11335,7 @@
         <v>0.3</v>
       </c>
       <c r="M212" s="5" t="s">
-        <v>2136</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="213" spans="1:13" x14ac:dyDescent="0.3">
@@ -11365,17 +11412,17 @@
         <v>941</v>
       </c>
       <c r="E217" s="2" t="s">
-        <v>2088</v>
+        <v>2080</v>
       </c>
       <c r="F217" s="2" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="G217" s="2">
         <v>13</v>
       </c>
       <c r="K217" s="27"/>
       <c r="M217" s="5" t="s">
-        <v>2087</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="218" spans="1:13" x14ac:dyDescent="0.3">
@@ -11620,7 +11667,7 @@
         <v>941</v>
       </c>
       <c r="E233" s="2" t="s">
-        <v>1973</v>
+        <v>1968</v>
       </c>
       <c r="K233" s="27"/>
     </row>
@@ -11638,7 +11685,7 @@
         <v>941</v>
       </c>
       <c r="E234" s="2" t="s">
-        <v>1973</v>
+        <v>1968</v>
       </c>
       <c r="K234" s="27"/>
     </row>
@@ -11686,7 +11733,7 @@
         <v>941</v>
       </c>
       <c r="E237" s="2" t="s">
-        <v>1974</v>
+        <v>1969</v>
       </c>
       <c r="K237" s="27"/>
     </row>
@@ -11704,7 +11751,7 @@
         <v>941</v>
       </c>
       <c r="E238" s="2" t="s">
-        <v>1973</v>
+        <v>1968</v>
       </c>
       <c r="K238" s="27"/>
     </row>
@@ -11755,7 +11802,7 @@
         <v>941</v>
       </c>
       <c r="E241" s="2" t="s">
-        <v>1973</v>
+        <v>1968</v>
       </c>
       <c r="K241" s="27"/>
     </row>
@@ -11927,7 +11974,7 @@
       </c>
       <c r="K251" s="27"/>
       <c r="M251" s="5" t="s">
-        <v>1980</v>
+        <v>1974</v>
       </c>
     </row>
     <row r="252" spans="1:13" x14ac:dyDescent="0.3">
@@ -12018,11 +12065,17 @@
       <c r="D257" s="2" t="s">
         <v>941</v>
       </c>
+      <c r="F257" s="2" t="s">
+        <v>2178</v>
+      </c>
+      <c r="G257" s="2">
+        <v>55</v>
+      </c>
       <c r="K257" s="27">
         <v>3.4</v>
       </c>
       <c r="M257" s="5" t="s">
-        <v>2124</v>
+        <v>2114</v>
       </c>
     </row>
     <row r="258" spans="1:13" x14ac:dyDescent="0.3">
@@ -12057,7 +12110,7 @@
         <v>1801</v>
       </c>
       <c r="F259" s="2" t="s">
-        <v>1989</v>
+        <v>1983</v>
       </c>
       <c r="G259" s="2">
         <v>51</v>
@@ -12067,7 +12120,7 @@
         <v>3.9527738679245283</v>
       </c>
       <c r="M259" s="5" t="s">
-        <v>2045</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="260" spans="1:13" x14ac:dyDescent="0.3">
@@ -12102,14 +12155,14 @@
         <v>1759</v>
       </c>
       <c r="F261" s="2" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="G261" s="2">
         <v>130</v>
       </c>
       <c r="K261" s="27"/>
       <c r="M261" s="5" t="s">
-        <v>2032</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="262" spans="1:13" x14ac:dyDescent="0.3">
@@ -12192,7 +12245,7 @@
         <v>1804</v>
       </c>
       <c r="F266" s="2" t="s">
-        <v>1988</v>
+        <v>1982</v>
       </c>
       <c r="G266" s="2">
         <v>101</v>
@@ -12202,7 +12255,7 @@
         <v>3.9667649043478264</v>
       </c>
       <c r="M266" s="5" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="267" spans="1:13" x14ac:dyDescent="0.3">
@@ -12289,7 +12342,7 @@
       </c>
       <c r="K271" s="27"/>
       <c r="M271" s="5" t="s">
-        <v>1960</v>
+        <v>1956</v>
       </c>
     </row>
     <row r="272" spans="1:13" x14ac:dyDescent="0.3">
@@ -12324,7 +12377,7 @@
         <v>1800</v>
       </c>
       <c r="F273" s="2" t="s">
-        <v>1988</v>
+        <v>1982</v>
       </c>
       <c r="G273" s="2">
         <v>580</v>
@@ -12334,7 +12387,7 @@
         <v>7.8397182185007974</v>
       </c>
       <c r="M273" s="5" t="s">
-        <v>2046</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="274" spans="1:13" x14ac:dyDescent="0.3">
@@ -12381,11 +12434,11 @@
         <v>941</v>
       </c>
       <c r="E276" s="2" t="s">
-        <v>2015</v>
+        <v>2007</v>
       </c>
       <c r="K276" s="27"/>
       <c r="M276" s="5" t="s">
-        <v>2071</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="277" spans="1:13" x14ac:dyDescent="0.3">
@@ -12451,7 +12504,7 @@
       </c>
       <c r="K280" s="27"/>
       <c r="M280" s="5" t="s">
-        <v>2020</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="281" spans="1:13" x14ac:dyDescent="0.3">
@@ -12654,14 +12707,14 @@
         <v>941</v>
       </c>
       <c r="E292" s="2" t="s">
-        <v>2163</v>
+        <v>2151</v>
       </c>
       <c r="G292" s="2">
         <v>13</v>
       </c>
       <c r="K292" s="27"/>
       <c r="M292" s="5" t="s">
-        <v>2164</v>
+        <v>2152</v>
       </c>
     </row>
     <row r="293" spans="1:13" x14ac:dyDescent="0.3">
@@ -12822,14 +12875,14 @@
         <v>1809</v>
       </c>
       <c r="F302" s="2" t="s">
-        <v>2119</v>
+        <v>2109</v>
       </c>
       <c r="G302" s="2">
         <v>25</v>
       </c>
       <c r="K302" s="27"/>
       <c r="M302" s="5" t="s">
-        <v>2120</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="303" spans="1:13" x14ac:dyDescent="0.3">
@@ -12886,7 +12939,7 @@
       </c>
       <c r="K305" s="27"/>
       <c r="M305" s="5" t="s">
-        <v>2067</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="306" spans="1:13" x14ac:dyDescent="0.3">
@@ -12906,11 +12959,11 @@
         <v>1757</v>
       </c>
       <c r="F306" s="2" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="K306" s="27"/>
       <c r="M306" s="5" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="307" spans="1:13" x14ac:dyDescent="0.3">
@@ -12930,11 +12983,11 @@
         <v>1757</v>
       </c>
       <c r="F307" s="2" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="K307" s="27"/>
       <c r="M307" s="5" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="308" spans="1:13" ht="75" x14ac:dyDescent="0.3">
@@ -12958,7 +13011,7 @@
       </c>
       <c r="K308" s="27"/>
       <c r="M308" s="5" t="s">
-        <v>2042</v>
+        <v>2034</v>
       </c>
     </row>
     <row r="309" spans="1:13" x14ac:dyDescent="0.3">
@@ -12991,7 +13044,7 @@
       </c>
       <c r="K310" s="27"/>
     </row>
-    <row r="311" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:13" ht="45" x14ac:dyDescent="0.3">
       <c r="A311" s="3">
         <v>2383</v>
       </c>
@@ -13004,11 +13057,17 @@
       <c r="D311" s="2" t="s">
         <v>941</v>
       </c>
+      <c r="E311" s="2" t="s">
+        <v>2185</v>
+      </c>
+      <c r="G311" s="2">
+        <v>140</v>
+      </c>
       <c r="K311" s="27">
         <v>7</v>
       </c>
       <c r="M311" s="5" t="s">
-        <v>2125</v>
+        <v>2186</v>
       </c>
     </row>
     <row r="312" spans="1:13" x14ac:dyDescent="0.3">
@@ -13026,7 +13085,7 @@
       </c>
       <c r="K312" s="27"/>
       <c r="M312" s="5" t="s">
-        <v>2074</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="313" spans="1:13" x14ac:dyDescent="0.3">
@@ -13166,7 +13225,7 @@
         <v>941</v>
       </c>
       <c r="E321" s="2" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="K321" s="27"/>
     </row>
@@ -13247,11 +13306,11 @@
         <v>941</v>
       </c>
       <c r="E326" s="2" t="s">
-        <v>2052</v>
+        <v>2044</v>
       </c>
       <c r="K326" s="27"/>
       <c r="M326" s="5" t="s">
-        <v>2053</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="327" spans="1:13" x14ac:dyDescent="0.3">
@@ -13272,7 +13331,7 @@
       </c>
       <c r="K327" s="27"/>
       <c r="M327" s="5" t="s">
-        <v>2025</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="328" spans="1:13" x14ac:dyDescent="0.3">
@@ -13292,11 +13351,11 @@
         <v>1802</v>
       </c>
       <c r="F328" s="2" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="K328" s="27"/>
       <c r="M328" s="5" t="s">
-        <v>2036</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="329" spans="1:13" x14ac:dyDescent="0.3">
@@ -13373,14 +13432,14 @@
         <v>1757</v>
       </c>
       <c r="F332" s="2" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="H332" s="2">
         <v>48</v>
       </c>
       <c r="K332" s="27"/>
       <c r="M332" s="5" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="333" spans="1:13" x14ac:dyDescent="0.3">
@@ -13613,17 +13672,17 @@
         <v>941</v>
       </c>
       <c r="E347" s="2" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="F347" s="4" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="G347" s="2">
         <v>41</v>
       </c>
       <c r="K347" s="27"/>
       <c r="M347" s="5" t="s">
-        <v>2089</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="348" spans="1:13" x14ac:dyDescent="0.3">
@@ -13748,10 +13807,10 @@
         <v>941</v>
       </c>
       <c r="E355" s="4" t="s">
-        <v>2090</v>
+        <v>2082</v>
       </c>
       <c r="F355" s="4" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="G355" s="2">
         <v>38</v>
@@ -13820,14 +13879,14 @@
         <v>1820</v>
       </c>
       <c r="F359" s="2" t="s">
-        <v>1988</v>
+        <v>1982</v>
       </c>
       <c r="K359" s="27"/>
       <c r="L359" s="24">
         <v>0.48331827758816837</v>
       </c>
       <c r="M359" s="5" t="s">
-        <v>2073</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="360" spans="1:13" x14ac:dyDescent="0.3">
@@ -13866,7 +13925,7 @@
       </c>
       <c r="K361" s="27"/>
       <c r="M361" s="5" t="s">
-        <v>1981</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="362" spans="1:13" x14ac:dyDescent="0.3">
@@ -13898,17 +13957,17 @@
         <v>941</v>
       </c>
       <c r="E363" s="2" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="F363" s="2" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="G363" s="2">
         <v>160</v>
       </c>
       <c r="K363" s="27"/>
       <c r="M363" s="5" t="s">
-        <v>2080</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="364" spans="1:13" x14ac:dyDescent="0.3">
@@ -13926,7 +13985,7 @@
       </c>
       <c r="K364" s="27"/>
       <c r="M364" s="5" t="s">
-        <v>2034</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="365" spans="1:13" x14ac:dyDescent="0.3">
@@ -14033,11 +14092,11 @@
         <v>941</v>
       </c>
       <c r="E371" s="2" t="s">
-        <v>1932</v>
+        <v>1929</v>
       </c>
       <c r="K371" s="27"/>
       <c r="M371" s="5" t="s">
-        <v>1933</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="372" spans="1:13" x14ac:dyDescent="0.3">
@@ -14075,7 +14134,7 @@
         <v>2472</v>
       </c>
       <c r="B374" s="1" t="s">
-        <v>1928</v>
+        <v>1926</v>
       </c>
       <c r="C374" s="2" t="s">
         <v>3</v>
@@ -14087,14 +14146,14 @@
         <v>1768</v>
       </c>
       <c r="F374" s="2" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="G374" s="2">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="K374" s="27"/>
       <c r="M374" s="5" t="s">
-        <v>2094</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="375" spans="1:13" x14ac:dyDescent="0.3">
@@ -14160,7 +14219,7 @@
       </c>
       <c r="K378" s="27"/>
       <c r="M378" s="5" t="s">
-        <v>1940</v>
+        <v>1937</v>
       </c>
     </row>
     <row r="379" spans="1:13" x14ac:dyDescent="0.3">
@@ -14195,14 +14254,14 @@
         <v>1768</v>
       </c>
       <c r="F380" s="2" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="G380" s="2">
         <v>50</v>
       </c>
       <c r="K380" s="27"/>
       <c r="M380" s="5" t="s">
-        <v>1982</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="381" spans="1:13" x14ac:dyDescent="0.3">
@@ -14279,7 +14338,7 @@
         <v>941</v>
       </c>
       <c r="E385" s="2" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="K385" s="27"/>
     </row>
@@ -14342,7 +14401,7 @@
         <v>941</v>
       </c>
       <c r="E389" s="4" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="G389" s="2">
         <v>220</v>
@@ -14576,7 +14635,7 @@
         <v>941</v>
       </c>
       <c r="E404" s="2" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="K404" s="27"/>
     </row>
@@ -14669,7 +14728,7 @@
         <v>941</v>
       </c>
       <c r="E410" s="2" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="K410" s="27"/>
     </row>
@@ -14807,10 +14866,10 @@
         <v>941</v>
       </c>
       <c r="E419" s="4" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="F419" s="2" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="G419" s="2">
         <v>46</v>
@@ -14846,7 +14905,7 @@
         <v>941</v>
       </c>
       <c r="E421" s="2" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="K421" s="27"/>
     </row>
@@ -15389,16 +15448,16 @@
         <v>941</v>
       </c>
       <c r="E457" s="2" t="s">
-        <v>2167</v>
+        <v>2155</v>
       </c>
       <c r="G457" s="2">
         <v>30</v>
       </c>
       <c r="K457" s="27" t="s">
-        <v>2165</v>
+        <v>2153</v>
       </c>
       <c r="M457" s="5" t="s">
-        <v>2166</v>
+        <v>2154</v>
       </c>
     </row>
     <row r="458" spans="1:13" x14ac:dyDescent="0.3">
@@ -15440,7 +15499,7 @@
       </c>
       <c r="K459" s="27"/>
       <c r="M459" s="5" t="s">
-        <v>2147</v>
+        <v>2135</v>
       </c>
     </row>
     <row r="460" spans="1:13" x14ac:dyDescent="0.3">
@@ -15503,7 +15562,7 @@
       </c>
       <c r="K463" s="27"/>
       <c r="M463" s="5" t="s">
-        <v>2063</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="464" spans="1:13" x14ac:dyDescent="0.3">
@@ -15731,7 +15790,7 @@
       </c>
       <c r="K477" s="27"/>
       <c r="M477" s="5" t="s">
-        <v>2049</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="478" spans="1:13" ht="30" x14ac:dyDescent="0.3">
@@ -15758,7 +15817,7 @@
       </c>
       <c r="K478" s="27"/>
       <c r="M478" s="5" t="s">
-        <v>2061</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="479" spans="1:13" x14ac:dyDescent="0.3">
@@ -15800,7 +15859,7 @@
       </c>
       <c r="K480" s="27"/>
       <c r="M480" s="5" t="s">
-        <v>2082</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="481" spans="1:13" ht="30" x14ac:dyDescent="0.3">
@@ -15827,7 +15886,7 @@
       </c>
       <c r="K481" s="27"/>
       <c r="M481" s="5" t="s">
-        <v>2060</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="482" spans="1:13" x14ac:dyDescent="0.3">
@@ -15902,7 +15961,7 @@
       </c>
       <c r="K485" s="27"/>
       <c r="M485" s="5" t="s">
-        <v>2056</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="486" spans="1:13" x14ac:dyDescent="0.3">
@@ -15935,7 +15994,7 @@
       </c>
       <c r="K487" s="27"/>
       <c r="M487" s="5" t="s">
-        <v>2023</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="488" spans="1:13" x14ac:dyDescent="0.3">
@@ -15953,7 +16012,7 @@
       </c>
       <c r="K488" s="27"/>
       <c r="M488" s="5" t="s">
-        <v>2028</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="489" spans="1:13" x14ac:dyDescent="0.3">
@@ -16015,7 +16074,7 @@
         <v>941</v>
       </c>
       <c r="E492" s="4" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="F492" s="2" t="s">
         <v>1767</v>
@@ -16121,7 +16180,7 @@
       </c>
       <c r="K498" s="27"/>
       <c r="M498" s="5" t="s">
-        <v>2024</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="499" spans="1:13" x14ac:dyDescent="0.3">
@@ -16244,7 +16303,7 @@
       </c>
       <c r="K506" s="27"/>
       <c r="M506" s="5" t="s">
-        <v>2079</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="507" spans="1:13" x14ac:dyDescent="0.3">
@@ -16276,16 +16335,16 @@
         <v>941</v>
       </c>
       <c r="E508" s="2" t="s">
-        <v>2168</v>
+        <v>2156</v>
       </c>
       <c r="G508" s="2">
         <v>45</v>
       </c>
       <c r="K508" s="27" t="s">
-        <v>2170</v>
+        <v>2158</v>
       </c>
       <c r="M508" s="5" t="s">
-        <v>2169</v>
+        <v>2157</v>
       </c>
     </row>
     <row r="509" spans="1:13" x14ac:dyDescent="0.3">
@@ -16328,7 +16387,7 @@
       </c>
       <c r="K510" s="27"/>
       <c r="M510" s="5" t="s">
-        <v>2047</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="511" spans="1:13" x14ac:dyDescent="0.3">
@@ -16394,7 +16453,7 @@
       </c>
       <c r="K514" s="27"/>
       <c r="M514" s="5" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="515" spans="1:13" x14ac:dyDescent="0.3">
@@ -16415,7 +16474,7 @@
       </c>
       <c r="K515" s="27"/>
       <c r="M515" s="5" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="516" spans="1:13" x14ac:dyDescent="0.3">
@@ -16451,7 +16510,7 @@
       </c>
       <c r="K517" s="27"/>
       <c r="M517" s="5" t="s">
-        <v>1942</v>
+        <v>1939</v>
       </c>
     </row>
     <row r="518" spans="1:13" x14ac:dyDescent="0.3">
@@ -16487,7 +16546,7 @@
       </c>
       <c r="K519" s="27"/>
       <c r="M519" s="5" t="s">
-        <v>2069</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="520" spans="1:13" x14ac:dyDescent="0.3">
@@ -16534,14 +16593,14 @@
         <v>941</v>
       </c>
       <c r="E522" s="4" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="G522" s="2">
         <v>160</v>
       </c>
       <c r="K522" s="27"/>
       <c r="M522" s="5" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="523" spans="1:13" x14ac:dyDescent="0.3">
@@ -16636,7 +16695,7 @@
         <v>941</v>
       </c>
       <c r="E528" s="2" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="G528" s="2">
         <v>36</v>
@@ -16717,14 +16776,14 @@
         <v>941</v>
       </c>
       <c r="E533" s="2" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="G533" s="2">
         <v>260</v>
       </c>
       <c r="K533" s="27"/>
       <c r="M533" s="5" t="s">
-        <v>2039</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="534" spans="1:13" x14ac:dyDescent="0.3">
@@ -16741,11 +16800,11 @@
         <v>941</v>
       </c>
       <c r="E534" s="2" t="s">
-        <v>2006</v>
+        <v>2000</v>
       </c>
       <c r="K534" s="27"/>
       <c r="M534" s="5" t="s">
-        <v>2048</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="535" spans="1:13" x14ac:dyDescent="0.3">
@@ -16763,7 +16822,7 @@
       </c>
       <c r="K535" s="27"/>
       <c r="M535" s="5" t="s">
-        <v>2075</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="536" spans="1:13" x14ac:dyDescent="0.3">
@@ -16790,7 +16849,7 @@
       </c>
       <c r="K536" s="27"/>
       <c r="M536" s="5" t="s">
-        <v>2027</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="537" spans="1:13" x14ac:dyDescent="0.3">
@@ -16841,7 +16900,7 @@
       </c>
       <c r="K539" s="27"/>
       <c r="M539" s="5" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="540" spans="1:13" x14ac:dyDescent="0.3">
@@ -16861,12 +16920,15 @@
         <v>1768</v>
       </c>
       <c r="F540" s="4" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="G540" s="2">
         <v>90</v>
       </c>
       <c r="K540" s="27"/>
+      <c r="M540" s="5" t="s">
+        <v>2167</v>
+      </c>
     </row>
     <row r="541" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A541" s="3">
@@ -16897,11 +16959,11 @@
         <v>941</v>
       </c>
       <c r="E542" s="2" t="s">
-        <v>2029</v>
+        <v>2021</v>
       </c>
       <c r="K542" s="27"/>
       <c r="M542" s="5" t="s">
-        <v>2030</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="543" spans="1:13" x14ac:dyDescent="0.3">
@@ -16921,11 +16983,11 @@
         <v>1802</v>
       </c>
       <c r="F543" s="2" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="K543" s="27"/>
       <c r="M543" s="5" t="s">
-        <v>2043</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="544" spans="1:13" x14ac:dyDescent="0.3">
@@ -17077,7 +17139,7 @@
         <v>941</v>
       </c>
       <c r="E553" s="2" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="K553" s="27"/>
     </row>
@@ -17185,10 +17247,10 @@
         <v>941</v>
       </c>
       <c r="K560" s="27" t="s">
-        <v>2153</v>
+        <v>2141</v>
       </c>
       <c r="M560" s="5" t="s">
-        <v>2152</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="561" spans="1:13" x14ac:dyDescent="0.3">
@@ -17254,7 +17316,7 @@
       </c>
       <c r="K564" s="27"/>
       <c r="M564" s="5" t="s">
-        <v>1929</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="565" spans="1:13" x14ac:dyDescent="0.3">
@@ -17302,7 +17364,7 @@
       </c>
       <c r="K567" s="27"/>
       <c r="M567" s="5" t="s">
-        <v>2059</v>
+        <v>2051</v>
       </c>
     </row>
     <row r="568" spans="1:13" x14ac:dyDescent="0.3">
@@ -17409,11 +17471,11 @@
         <v>941</v>
       </c>
       <c r="E574" s="2" t="s">
-        <v>2108</v>
+        <v>2098</v>
       </c>
       <c r="K574" s="27"/>
       <c r="M574" s="5" t="s">
-        <v>2109</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="575" spans="1:13" x14ac:dyDescent="0.3">
@@ -17490,7 +17552,7 @@
         <v>941</v>
       </c>
       <c r="E579" s="2" t="s">
-        <v>1967</v>
+        <v>1963</v>
       </c>
       <c r="K579" s="27"/>
     </row>
@@ -17570,11 +17632,20 @@
       <c r="D584" s="2" t="s">
         <v>941</v>
       </c>
+      <c r="E584" s="2" t="s">
+        <v>2180</v>
+      </c>
+      <c r="F584" s="2" t="s">
+        <v>2178</v>
+      </c>
+      <c r="G584" s="2">
+        <v>72</v>
+      </c>
       <c r="K584" s="27">
         <v>4</v>
       </c>
       <c r="M584" s="5" t="s">
-        <v>2126</v>
+        <v>2115</v>
       </c>
     </row>
     <row r="585" spans="1:13" x14ac:dyDescent="0.3">
@@ -17688,7 +17759,7 @@
       </c>
       <c r="K591" s="27"/>
       <c r="M591" s="5" t="s">
-        <v>2026</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="592" spans="1:13" x14ac:dyDescent="0.3">
@@ -17754,7 +17825,7 @@
       </c>
       <c r="K595" s="27"/>
       <c r="M595" s="5" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="596" spans="1:13" x14ac:dyDescent="0.3">
@@ -17841,7 +17912,7 @@
       </c>
       <c r="K600" s="27"/>
       <c r="M600" s="5" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="601" spans="1:13" x14ac:dyDescent="0.3">
@@ -17949,7 +18020,7 @@
       </c>
       <c r="K607" s="27"/>
       <c r="M607" s="5" t="s">
-        <v>2081</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="608" spans="1:13" x14ac:dyDescent="0.3">
@@ -18069,7 +18140,7 @@
       </c>
       <c r="K614" s="27"/>
       <c r="M614" s="5" t="s">
-        <v>1959</v>
+        <v>1955</v>
       </c>
     </row>
     <row r="615" spans="1:13" x14ac:dyDescent="0.3">
@@ -18146,7 +18217,7 @@
         <v>941</v>
       </c>
       <c r="E619" s="2" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="G619" s="2">
         <v>160</v>
@@ -18176,7 +18247,7 @@
         <v>3665</v>
       </c>
       <c r="B621" s="1" t="s">
-        <v>1986</v>
+        <v>1980</v>
       </c>
       <c r="C621" s="2" t="s">
         <v>3</v>
@@ -18189,7 +18260,7 @@
       </c>
       <c r="K621" s="27"/>
       <c r="M621" s="5" t="s">
-        <v>1953</v>
+        <v>1949</v>
       </c>
     </row>
     <row r="622" spans="1:13" x14ac:dyDescent="0.3">
@@ -18209,7 +18280,7 @@
         <v>1757</v>
       </c>
       <c r="F622" s="2" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="H622" s="2">
         <v>70</v>
@@ -18230,11 +18301,11 @@
         <v>941</v>
       </c>
       <c r="E623" s="2" t="s">
-        <v>2018</v>
+        <v>2010</v>
       </c>
       <c r="K623" s="27"/>
       <c r="M623" s="5" t="s">
-        <v>2019</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="624" spans="1:13" x14ac:dyDescent="0.3">
@@ -18251,14 +18322,17 @@
         <v>941</v>
       </c>
       <c r="E624" s="2" t="s">
-        <v>2099</v>
+        <v>2090</v>
       </c>
       <c r="F624" s="2" t="s">
-        <v>2101</v>
+        <v>1900</v>
+      </c>
+      <c r="H624" s="2">
+        <v>120</v>
       </c>
       <c r="K624" s="27"/>
       <c r="M624" s="5" t="s">
-        <v>2100</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="625" spans="1:13" x14ac:dyDescent="0.3">
@@ -18371,14 +18445,14 @@
         <v>941</v>
       </c>
       <c r="E631" s="2" t="s">
-        <v>2091</v>
+        <v>2083</v>
       </c>
       <c r="G631" s="2">
         <v>31</v>
       </c>
       <c r="K631" s="27"/>
       <c r="M631" s="5" t="s">
-        <v>1935</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="632" spans="1:13" x14ac:dyDescent="0.3">
@@ -18447,7 +18521,7 @@
       </c>
       <c r="K635" s="27"/>
       <c r="M635" s="5" t="s">
-        <v>2022</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="636" spans="1:13" x14ac:dyDescent="0.3">
@@ -18479,17 +18553,17 @@
         <v>941</v>
       </c>
       <c r="E637" s="4" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="F637" s="2" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="G637" s="2">
         <v>48</v>
       </c>
       <c r="K637" s="27"/>
       <c r="M637" s="5" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="638" spans="1:13" x14ac:dyDescent="0.3">
@@ -18536,7 +18610,7 @@
         <v>941</v>
       </c>
       <c r="E640" s="4" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="G640" s="2">
         <v>80</v>
@@ -18602,11 +18676,11 @@
         <v>941</v>
       </c>
       <c r="E644" s="4" t="s">
-        <v>1920</v>
+        <v>1918</v>
       </c>
       <c r="K644" s="27"/>
       <c r="M644" s="5" t="s">
-        <v>1921</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="645" spans="1:13" x14ac:dyDescent="0.3">
@@ -18683,16 +18757,16 @@
         <v>941</v>
       </c>
       <c r="E649" s="2" t="s">
-        <v>2173</v>
+        <v>2161</v>
       </c>
       <c r="F649" s="2" t="s">
-        <v>2154</v>
+        <v>2142</v>
       </c>
       <c r="K649" s="27" t="s">
-        <v>2171</v>
+        <v>2159</v>
       </c>
       <c r="M649" s="5" t="s">
-        <v>2172</v>
+        <v>2160</v>
       </c>
     </row>
     <row r="650" spans="1:13" x14ac:dyDescent="0.3">
@@ -18850,7 +18924,7 @@
         <v>941</v>
       </c>
       <c r="E659" s="2" t="s">
-        <v>2174</v>
+        <v>2162</v>
       </c>
       <c r="K659" s="27"/>
     </row>
@@ -18973,14 +19047,14 @@
         <v>941</v>
       </c>
       <c r="E667" s="2" t="s">
-        <v>2031</v>
+        <v>2023</v>
       </c>
       <c r="G667" s="2">
         <v>80</v>
       </c>
       <c r="K667" s="27"/>
       <c r="M667" s="5" t="s">
-        <v>2111</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="668" spans="1:13" x14ac:dyDescent="0.3">
@@ -19012,7 +19086,7 @@
         <v>941</v>
       </c>
       <c r="E669" s="2" t="s">
-        <v>1976</v>
+        <v>1971</v>
       </c>
       <c r="K669" s="27"/>
     </row>
@@ -19090,13 +19164,13 @@
         <v>941</v>
       </c>
       <c r="E674" s="2" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="K674" s="27" t="s">
-        <v>2159</v>
+        <v>2147</v>
       </c>
       <c r="M674" s="5" t="s">
-        <v>2175</v>
+        <v>2163</v>
       </c>
     </row>
     <row r="675" spans="1:13" x14ac:dyDescent="0.3">
@@ -19114,7 +19188,7 @@
       </c>
       <c r="K675" s="27"/>
       <c r="M675" s="5" t="s">
-        <v>2114</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="676" spans="1:13" x14ac:dyDescent="0.3">
@@ -19194,11 +19268,11 @@
         <v>1802</v>
       </c>
       <c r="F680" s="2" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="K680" s="27"/>
       <c r="M680" s="5" t="s">
-        <v>2044</v>
+        <v>2036</v>
       </c>
     </row>
     <row r="681" spans="1:13" x14ac:dyDescent="0.3">
@@ -19234,7 +19308,7 @@
       </c>
       <c r="K682" s="27"/>
       <c r="M682" s="5" t="s">
-        <v>2176</v>
+        <v>2164</v>
       </c>
     </row>
     <row r="683" spans="1:13" x14ac:dyDescent="0.3">
@@ -19251,7 +19325,7 @@
         <v>941</v>
       </c>
       <c r="E683" s="2" t="s">
-        <v>2000</v>
+        <v>1994</v>
       </c>
       <c r="G683" s="2">
         <v>54</v>
@@ -19288,7 +19362,7 @@
       </c>
       <c r="K685" s="27"/>
     </row>
-    <row r="686" spans="1:13" ht="30" x14ac:dyDescent="0.3">
+    <row r="686" spans="1:13" ht="45" x14ac:dyDescent="0.3">
       <c r="A686" s="3">
         <v>4927</v>
       </c>
@@ -19301,14 +19375,17 @@
       <c r="D686" s="2" t="s">
         <v>941</v>
       </c>
+      <c r="E686" s="2" t="s">
+        <v>2183</v>
+      </c>
       <c r="G686" s="2">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="K686" s="27" t="s">
-        <v>2150</v>
+        <v>2138</v>
       </c>
       <c r="M686" s="5" t="s">
-        <v>2177</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="687" spans="1:13" x14ac:dyDescent="0.3">
@@ -19362,7 +19439,7 @@
       </c>
       <c r="K689" s="27"/>
       <c r="M689" s="5" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="690" spans="1:13" x14ac:dyDescent="0.3">
@@ -19509,7 +19586,7 @@
       </c>
       <c r="K698" s="27"/>
       <c r="M698" s="5" t="s">
-        <v>1954</v>
+        <v>1950</v>
       </c>
     </row>
     <row r="699" spans="1:13" ht="60" x14ac:dyDescent="0.3">
@@ -19526,14 +19603,14 @@
         <v>941</v>
       </c>
       <c r="E699" s="2" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="G699" s="2">
         <v>200</v>
       </c>
       <c r="K699" s="27"/>
       <c r="M699" s="5" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="700" spans="1:13" x14ac:dyDescent="0.3">
@@ -19616,11 +19693,11 @@
         <v>941</v>
       </c>
       <c r="E704" s="2" t="s">
-        <v>1967</v>
+        <v>1963</v>
       </c>
       <c r="K704" s="27"/>
       <c r="M704" s="5" t="s">
-        <v>2016</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="705" spans="1:13" x14ac:dyDescent="0.3">
@@ -19757,7 +19834,7 @@
         <v>941</v>
       </c>
       <c r="E712" s="2" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="K712" s="27"/>
     </row>
@@ -19877,14 +19954,14 @@
         <v>941</v>
       </c>
       <c r="E719" s="2" t="s">
-        <v>2104</v>
+        <v>2094</v>
       </c>
       <c r="G719" s="2">
         <v>40</v>
       </c>
       <c r="K719" s="27"/>
       <c r="M719" s="5" t="s">
-        <v>2106</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="720" spans="1:13" x14ac:dyDescent="0.3">
@@ -20036,7 +20113,7 @@
         <v>941</v>
       </c>
       <c r="E729" s="2" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="K729" s="27"/>
     </row>
@@ -20114,17 +20191,17 @@
         <v>941</v>
       </c>
       <c r="E734" s="4" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="F734" s="2" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="G734" s="2">
         <v>110</v>
       </c>
       <c r="K734" s="27"/>
       <c r="M734" s="5" t="s">
-        <v>2115</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="735" spans="1:13" x14ac:dyDescent="0.3">
@@ -20246,10 +20323,10 @@
         <v>941</v>
       </c>
       <c r="E742" s="2" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="F742" s="2" t="s">
-        <v>1983</v>
+        <v>1977</v>
       </c>
       <c r="G742" s="2">
         <v>41</v>
@@ -20258,7 +20335,7 @@
         <v>2.5</v>
       </c>
       <c r="M742" s="5" t="s">
-        <v>2127</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="743" spans="1:13" x14ac:dyDescent="0.3">
@@ -20446,7 +20523,7 @@
         <v>941</v>
       </c>
       <c r="E754" s="4" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="F754" s="2" t="s">
         <v>1764</v>
@@ -20456,7 +20533,7 @@
       </c>
       <c r="K754" s="27"/>
       <c r="M754" s="5" t="s">
-        <v>2112</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="755" spans="1:13" x14ac:dyDescent="0.3">
@@ -20593,7 +20670,7 @@
         <v>941</v>
       </c>
       <c r="E763" s="2" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="F763" s="2" t="s">
         <v>1767</v>
@@ -20650,14 +20727,14 @@
         <v>941</v>
       </c>
       <c r="E766" s="4" t="s">
-        <v>2102</v>
+        <v>2092</v>
       </c>
       <c r="G766" s="2">
         <v>24.1</v>
       </c>
       <c r="K766" s="27"/>
       <c r="M766" s="5" t="s">
-        <v>2103</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="767" spans="1:13" x14ac:dyDescent="0.3">
@@ -20718,17 +20795,17 @@
       <c r="D770" s="2" t="s">
         <v>941</v>
       </c>
-      <c r="F770" s="2" t="s">
-        <v>2180</v>
+      <c r="E770" s="2" t="s">
+        <v>1858</v>
       </c>
       <c r="G770" s="2">
         <v>80</v>
       </c>
       <c r="K770" s="27" t="s">
-        <v>2178</v>
+        <v>2165</v>
       </c>
       <c r="M770" s="5" t="s">
-        <v>2179</v>
+        <v>2166</v>
       </c>
     </row>
     <row r="771" spans="1:13" ht="60" x14ac:dyDescent="0.3">
@@ -20748,14 +20825,14 @@
         <v>1819</v>
       </c>
       <c r="F771" s="2" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="G771" s="2">
         <v>41</v>
       </c>
       <c r="K771" s="27"/>
       <c r="M771" s="5" t="s">
-        <v>2092</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="772" spans="1:13" x14ac:dyDescent="0.3">
@@ -20821,7 +20898,7 @@
       </c>
       <c r="K775" s="27"/>
       <c r="M775" s="5" t="s">
-        <v>2040</v>
+        <v>2032</v>
       </c>
     </row>
     <row r="776" spans="1:13" x14ac:dyDescent="0.3">
@@ -20868,14 +20945,14 @@
         <v>941</v>
       </c>
       <c r="E778" s="2" t="s">
-        <v>1969</v>
-      </c>
-      <c r="F778" s="2" t="s">
-        <v>1970</v>
+        <v>1965</v>
+      </c>
+      <c r="G778" s="2">
+        <v>75</v>
       </c>
       <c r="K778" s="27"/>
       <c r="M778" s="5" t="s">
-        <v>1971</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="779" spans="1:13" x14ac:dyDescent="0.3">
@@ -20926,7 +21003,7 @@
       </c>
       <c r="K781" s="27"/>
       <c r="M781" s="5" t="s">
-        <v>1943</v>
+        <v>1940</v>
       </c>
     </row>
     <row r="782" spans="1:13" x14ac:dyDescent="0.3">
@@ -20946,7 +21023,7 @@
         <v>0.6</v>
       </c>
       <c r="M782" s="5" t="s">
-        <v>2128</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="783" spans="1:13" x14ac:dyDescent="0.3">
@@ -21033,7 +21110,7 @@
       </c>
       <c r="K787" s="27"/>
       <c r="M787" s="5" t="s">
-        <v>2066</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="788" spans="1:13" ht="90" x14ac:dyDescent="0.3">
@@ -21230,10 +21307,10 @@
         <v>941</v>
       </c>
       <c r="K799" s="27" t="s">
-        <v>2144</v>
+        <v>2132</v>
       </c>
       <c r="M799" s="5" t="s">
-        <v>2146</v>
+        <v>2134</v>
       </c>
     </row>
     <row r="800" spans="1:13" x14ac:dyDescent="0.3">
@@ -21250,7 +21327,7 @@
         <v>941</v>
       </c>
       <c r="E800" s="2" t="s">
-        <v>1975</v>
+        <v>1970</v>
       </c>
       <c r="K800" s="27"/>
     </row>
@@ -21268,7 +21345,7 @@
         <v>941</v>
       </c>
       <c r="E801" s="2" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="K801" s="27"/>
     </row>
@@ -21286,7 +21363,7 @@
         <v>941</v>
       </c>
       <c r="E802" s="2" t="s">
-        <v>1975</v>
+        <v>1970</v>
       </c>
       <c r="K802" s="27"/>
     </row>
@@ -21320,7 +21397,7 @@
       </c>
       <c r="K804" s="27"/>
     </row>
-    <row r="805" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="805" spans="1:13" ht="30" x14ac:dyDescent="0.3">
       <c r="A805" s="3">
         <v>6443</v>
       </c>
@@ -21337,14 +21414,13 @@
         <v>1710</v>
       </c>
       <c r="F805" s="2" t="s">
-        <v>1901</v>
-      </c>
-      <c r="G805" s="2">
-        <v>32</v>
-      </c>
-      <c r="K805" s="27"/>
+        <v>2170</v>
+      </c>
+      <c r="K805" s="27" t="s">
+        <v>2168</v>
+      </c>
       <c r="M805" s="5" t="s">
-        <v>2095</v>
+        <v>2169</v>
       </c>
     </row>
     <row r="806" spans="1:13" x14ac:dyDescent="0.3">
@@ -21442,13 +21518,13 @@
         <v>941</v>
       </c>
       <c r="E811" s="2" t="s">
-        <v>2041</v>
+        <v>2033</v>
       </c>
       <c r="K811" s="27">
         <v>5</v>
       </c>
       <c r="M811" s="5" t="s">
-        <v>2129</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="812" spans="1:13" x14ac:dyDescent="0.3">
@@ -21480,11 +21556,11 @@
         <v>941</v>
       </c>
       <c r="E813" s="2" t="s">
-        <v>2050</v>
+        <v>2042</v>
       </c>
       <c r="K813" s="27"/>
       <c r="M813" s="5" t="s">
-        <v>2055</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="814" spans="1:13" x14ac:dyDescent="0.3">
@@ -21608,6 +21684,9 @@
       <c r="D821" s="2" t="s">
         <v>941</v>
       </c>
+      <c r="E821" s="2" t="s">
+        <v>2180</v>
+      </c>
       <c r="K821" s="27"/>
     </row>
     <row r="822" spans="1:13" x14ac:dyDescent="0.3">
@@ -21624,13 +21703,13 @@
         <v>941</v>
       </c>
       <c r="E822" s="2" t="s">
-        <v>2033</v>
+        <v>2025</v>
       </c>
       <c r="K822" s="27">
         <v>3</v>
       </c>
       <c r="M822" s="5" t="s">
-        <v>2130</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="823" spans="1:13" x14ac:dyDescent="0.3">
@@ -21686,7 +21765,7 @@
         <v>941</v>
       </c>
       <c r="E825" s="4" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="G825" s="2">
         <v>50</v>
@@ -21707,7 +21786,7 @@
         <v>941</v>
       </c>
       <c r="E826" s="2" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="K826" s="27"/>
     </row>
@@ -21819,7 +21898,7 @@
       </c>
       <c r="K833" s="27"/>
       <c r="M833" s="5" t="s">
-        <v>2064</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="834" spans="1:13" x14ac:dyDescent="0.3">
@@ -21921,7 +22000,7 @@
       </c>
       <c r="K839" s="27"/>
       <c r="M839" s="5" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="840" spans="1:13" x14ac:dyDescent="0.3">
@@ -21998,10 +22077,10 @@
         <v>941</v>
       </c>
       <c r="E844" s="4" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="F844" s="2" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="G844" s="2">
         <v>28</v>
@@ -22010,7 +22089,7 @@
         <v>1.58</v>
       </c>
       <c r="M844" s="26" t="s">
-        <v>2131</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="845" spans="1:13" x14ac:dyDescent="0.3">
@@ -22018,7 +22097,7 @@
         <v>8028</v>
       </c>
       <c r="B845" s="3" t="s">
-        <v>1957</v>
+        <v>1953</v>
       </c>
       <c r="C845" s="2" t="s">
         <v>3</v>
@@ -22084,7 +22163,7 @@
         <v>3.4</v>
       </c>
       <c r="M848" s="5" t="s">
-        <v>2132</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="849" spans="1:13" ht="30" x14ac:dyDescent="0.3">
@@ -22101,14 +22180,14 @@
         <v>941</v>
       </c>
       <c r="E849" s="2" t="s">
-        <v>2001</v>
+        <v>1995</v>
       </c>
       <c r="F849" s="2" t="s">
-        <v>2003</v>
+        <v>1997</v>
       </c>
       <c r="K849" s="27"/>
       <c r="M849" s="5" t="s">
-        <v>2002</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="850" spans="1:13" x14ac:dyDescent="0.3">
@@ -22140,11 +22219,11 @@
         <v>941</v>
       </c>
       <c r="E851" s="2" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="K851" s="27"/>
       <c r="M851" s="5" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="852" spans="1:13" x14ac:dyDescent="0.3">
@@ -22449,14 +22528,14 @@
         <v>941</v>
       </c>
       <c r="E871" s="2" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="F871" s="2" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="K871" s="27"/>
       <c r="M871" s="5" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="872" spans="1:13" x14ac:dyDescent="0.3">
@@ -22593,17 +22672,17 @@
         <v>941</v>
       </c>
       <c r="E880" s="2" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="F880" s="2" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="G880" s="2">
         <v>320</v>
       </c>
       <c r="K880" s="27"/>
       <c r="M880" s="5" t="s">
-        <v>2068</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="881" spans="1:13" x14ac:dyDescent="0.3">
@@ -22680,10 +22759,10 @@
         <v>941</v>
       </c>
       <c r="K885" s="27" t="s">
-        <v>2149</v>
+        <v>2137</v>
       </c>
       <c r="M885" s="5" t="s">
-        <v>2148</v>
+        <v>2136</v>
       </c>
     </row>
     <row r="886" spans="1:13" x14ac:dyDescent="0.3">
@@ -22794,7 +22873,7 @@
       </c>
       <c r="K892" s="27"/>
       <c r="M892" s="5" t="s">
-        <v>1944</v>
+        <v>1941</v>
       </c>
     </row>
     <row r="893" spans="1:13" x14ac:dyDescent="0.3">
@@ -23051,13 +23130,16 @@
         <v>941</v>
       </c>
       <c r="E909" s="2" t="s">
-        <v>2110</v>
+        <v>2100</v>
+      </c>
+      <c r="G909" s="2">
+        <v>72</v>
       </c>
       <c r="K909" s="27">
         <v>3.8</v>
       </c>
       <c r="M909" s="5" t="s">
-        <v>2133</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="910" spans="1:13" x14ac:dyDescent="0.3">
@@ -23260,11 +23342,11 @@
         <v>1815</v>
       </c>
       <c r="F922" s="2" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="K922" s="27"/>
       <c r="M922" s="5" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="923" spans="1:13" x14ac:dyDescent="0.3">
@@ -23299,7 +23381,7 @@
         <v>941</v>
       </c>
       <c r="E924" s="2" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="F924" s="2" t="s">
         <v>1767</v>
@@ -23309,7 +23391,7 @@
       </c>
       <c r="K924" s="27"/>
       <c r="M924" s="5" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="925" spans="1:13" x14ac:dyDescent="0.3">
@@ -23477,7 +23559,7 @@
       </c>
       <c r="K935" s="27"/>
     </row>
-    <row r="936" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="936" spans="1:13" ht="45" x14ac:dyDescent="0.3">
       <c r="A936" s="3">
         <v>9938</v>
       </c>
@@ -23491,17 +23573,17 @@
         <v>941</v>
       </c>
       <c r="E936" s="2" t="s">
-        <v>1978</v>
+        <v>1973</v>
       </c>
       <c r="F936" s="2" t="s">
-        <v>2096</v>
+        <v>2087</v>
       </c>
       <c r="G936" s="2">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="K936" s="27"/>
       <c r="M936" s="5" t="s">
-        <v>1979</v>
+        <v>2171</v>
       </c>
     </row>
     <row r="937" spans="1:13" x14ac:dyDescent="0.3">
@@ -23548,10 +23630,10 @@
         <v>941</v>
       </c>
       <c r="E939" s="4" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="F939" s="2" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="G939" s="2">
         <v>95</v>
@@ -23587,17 +23669,17 @@
         <v>941</v>
       </c>
       <c r="E941" s="4" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="F941" s="2" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="G941" s="2">
         <v>55</v>
       </c>
       <c r="K941" s="27"/>
       <c r="M941" s="5" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="942" spans="1:13" x14ac:dyDescent="0.3">
@@ -23681,7 +23763,7 @@
       </c>
       <c r="K946" s="27"/>
       <c r="M946" s="5" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="947" spans="1:13" x14ac:dyDescent="0.3">
@@ -23849,7 +23931,7 @@
       </c>
       <c r="K957" s="27"/>
       <c r="M957" s="5" t="s">
-        <v>2062</v>
+        <v>2054</v>
       </c>
     </row>
     <row r="958" spans="1:13" ht="45" x14ac:dyDescent="0.3">
@@ -23857,7 +23939,7 @@
         <v>1586</v>
       </c>
       <c r="B958" s="1" t="s">
-        <v>1987</v>
+        <v>1981</v>
       </c>
       <c r="C958" s="2" t="s">
         <v>1701</v>
@@ -23869,14 +23951,14 @@
         <v>1819</v>
       </c>
       <c r="F958" s="2" t="s">
-        <v>2093</v>
+        <v>2085</v>
       </c>
       <c r="G958" s="2">
         <v>41</v>
       </c>
       <c r="K958" s="27"/>
       <c r="M958" s="5" t="s">
-        <v>1964</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="959" spans="1:13" x14ac:dyDescent="0.3">
@@ -23944,7 +24026,7 @@
         <v>1.5</v>
       </c>
       <c r="M962" s="5" t="s">
-        <v>2023</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="963" spans="1:13" x14ac:dyDescent="0.3">
@@ -24006,14 +24088,14 @@
         <v>941</v>
       </c>
       <c r="E966" s="2" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="G966" s="2">
         <v>70</v>
       </c>
       <c r="K966" s="27"/>
       <c r="M966" s="5" t="s">
-        <v>1945</v>
+        <v>1942</v>
       </c>
     </row>
     <row r="967" spans="1:13" x14ac:dyDescent="0.3">
@@ -24084,7 +24166,7 @@
         <v>941</v>
       </c>
       <c r="E970" s="2" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="F970" s="2" t="s">
         <v>1767</v>
@@ -24094,7 +24176,7 @@
       </c>
       <c r="K970" s="27"/>
       <c r="M970" s="5" t="s">
-        <v>1947</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="971" spans="1:13" x14ac:dyDescent="0.3">
@@ -24217,7 +24299,7 @@
       </c>
       <c r="K978" s="27"/>
     </row>
-    <row r="979" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="979" spans="1:13" ht="30" x14ac:dyDescent="0.3">
       <c r="A979" s="3">
         <v>2065</v>
       </c>
@@ -24231,19 +24313,19 @@
         <v>941</v>
       </c>
       <c r="E979" s="2" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="F979" s="2" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="G979" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K979" s="27">
         <v>3</v>
       </c>
       <c r="M979" s="5" t="s">
-        <v>2134</v>
+        <v>2179</v>
       </c>
     </row>
     <row r="980" spans="1:13" x14ac:dyDescent="0.3">
@@ -24395,11 +24477,11 @@
         <v>941</v>
       </c>
       <c r="E989" s="2" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="K989" s="27"/>
       <c r="M989" s="5" t="s">
-        <v>1925</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="990" spans="1:13" x14ac:dyDescent="0.3">
@@ -24582,7 +24664,7 @@
       </c>
       <c r="K1001" s="27"/>
       <c r="M1001" s="5" t="s">
-        <v>2151</v>
+        <v>2139</v>
       </c>
     </row>
     <row r="1002" spans="1:13" x14ac:dyDescent="0.3">
@@ -24755,7 +24837,7 @@
         <v>941</v>
       </c>
       <c r="E1012" s="4" t="s">
-        <v>1984</v>
+        <v>1978</v>
       </c>
       <c r="H1012" s="2">
         <v>50</v>
@@ -24861,7 +24943,7 @@
       </c>
       <c r="K1018" s="27"/>
       <c r="M1018" s="5" t="s">
-        <v>1958</v>
+        <v>1954</v>
       </c>
     </row>
     <row r="1019" spans="1:13" x14ac:dyDescent="0.3">
@@ -24911,11 +24993,11 @@
         <v>941</v>
       </c>
       <c r="E1021" s="2" t="s">
-        <v>2011</v>
+        <v>2004</v>
       </c>
       <c r="K1021" s="27"/>
       <c r="M1021" s="5" t="s">
-        <v>2038</v>
+        <v>2030</v>
       </c>
     </row>
     <row r="1022" spans="1:13" x14ac:dyDescent="0.3">
@@ -24989,7 +25071,7 @@
         <v>3128</v>
       </c>
       <c r="B1026" s="1" t="s">
-        <v>2078</v>
+        <v>2070</v>
       </c>
       <c r="C1026" s="2" t="s">
         <v>1701</v>
@@ -25148,7 +25230,7 @@
         <v>941</v>
       </c>
       <c r="E1036" s="2" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="K1036" s="27"/>
     </row>
@@ -25251,7 +25333,7 @@
       </c>
       <c r="K1042" s="27"/>
       <c r="M1042" s="5" t="s">
-        <v>1963</v>
+        <v>1959</v>
       </c>
     </row>
     <row r="1043" spans="1:13" x14ac:dyDescent="0.3">
@@ -25338,7 +25420,7 @@
       </c>
       <c r="K1047" s="27"/>
       <c r="M1047" s="5" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="1048" spans="1:13" x14ac:dyDescent="0.3">
@@ -25430,7 +25512,7 @@
         <v>941</v>
       </c>
       <c r="E1053" s="2" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="G1053" s="2">
         <v>240</v>
@@ -25544,14 +25626,14 @@
         <v>1826</v>
       </c>
       <c r="F1060" s="2" t="s">
-        <v>2093</v>
+        <v>2085</v>
       </c>
       <c r="G1060" s="2">
         <v>66</v>
       </c>
       <c r="K1060" s="27"/>
       <c r="M1060" s="5" t="s">
-        <v>2021</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="1061" spans="1:14" x14ac:dyDescent="0.3">
@@ -25616,7 +25698,7 @@
         <v>1757</v>
       </c>
       <c r="F1064" s="2" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="K1064" s="27"/>
       <c r="M1064" s="7" t="s">
@@ -25713,7 +25795,7 @@
       </c>
       <c r="K1070" s="27"/>
       <c r="M1070" s="5" t="s">
-        <v>2076</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="1071" spans="1:14" x14ac:dyDescent="0.3">
@@ -25748,7 +25830,7 @@
         <v>1780</v>
       </c>
       <c r="F1072" s="2" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="G1072" s="2">
         <v>750</v>
@@ -25757,13 +25839,13 @@
         <v>752</v>
       </c>
       <c r="K1072" s="27" t="s">
-        <v>2142</v>
+        <v>2130</v>
       </c>
       <c r="M1072" s="7" t="s">
-        <v>2084</v>
+        <v>2076</v>
       </c>
       <c r="N1072" s="25" t="s">
-        <v>2005</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="1073" spans="1:13" x14ac:dyDescent="0.3">
@@ -25918,14 +26000,14 @@
         <v>1712</v>
       </c>
       <c r="F1082" s="2" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="I1082" s="2">
         <v>225</v>
       </c>
       <c r="K1082" s="27"/>
       <c r="M1082" s="5" t="s">
-        <v>2085</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="1083" spans="1:13" x14ac:dyDescent="0.3">
@@ -26002,14 +26084,14 @@
         <v>941</v>
       </c>
       <c r="E1087" s="4" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="F1087" s="2" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="K1087" s="27"/>
       <c r="M1087" s="5" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="1088" spans="1:13" x14ac:dyDescent="0.3">
@@ -26375,7 +26457,7 @@
       </c>
       <c r="K1110" s="27"/>
       <c r="M1110" s="5" t="s">
-        <v>2065</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="1111" spans="1:13" x14ac:dyDescent="0.3">
@@ -26543,7 +26625,7 @@
       </c>
       <c r="K1121" s="27"/>
     </row>
-    <row r="1122" spans="1:13" ht="30" x14ac:dyDescent="0.3">
+    <row r="1122" spans="1:13" ht="45" x14ac:dyDescent="0.3">
       <c r="A1122" s="3">
         <v>3526</v>
       </c>
@@ -26557,7 +26639,7 @@
         <v>941</v>
       </c>
       <c r="E1122" s="2" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="F1122" s="2" t="s">
         <v>1767</v>
@@ -26565,9 +26647,11 @@
       <c r="G1122" s="2">
         <v>80</v>
       </c>
-      <c r="K1122" s="27"/>
+      <c r="K1122" s="27" t="s">
+        <v>2188</v>
+      </c>
       <c r="M1122" s="5" t="s">
-        <v>1913</v>
+        <v>2187</v>
       </c>
     </row>
     <row r="1123" spans="1:13" x14ac:dyDescent="0.3">
@@ -26680,14 +26764,14 @@
         <v>1780</v>
       </c>
       <c r="F1129" s="2" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="G1129" s="2">
         <v>81</v>
       </c>
       <c r="K1129" s="27"/>
       <c r="M1129" s="5" t="s">
-        <v>1914</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="1130" spans="1:13" x14ac:dyDescent="0.3">
@@ -26720,7 +26804,7 @@
       </c>
       <c r="K1131" s="27"/>
     </row>
-    <row r="1132" spans="1:13" ht="60" x14ac:dyDescent="0.3">
+    <row r="1132" spans="1:13" ht="45" x14ac:dyDescent="0.3">
       <c r="A1132" s="3">
         <v>3552</v>
       </c>
@@ -26737,14 +26821,14 @@
         <v>1819</v>
       </c>
       <c r="F1132" s="2" t="s">
-        <v>1906</v>
+        <v>2173</v>
       </c>
       <c r="G1132" s="2">
         <v>250</v>
       </c>
       <c r="K1132" s="27"/>
       <c r="M1132" s="7" t="s">
-        <v>1948</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="1133" spans="1:13" x14ac:dyDescent="0.3">
@@ -26887,7 +26971,7 @@
         <v>3587</v>
       </c>
       <c r="B1142" s="1" t="s">
-        <v>2012</v>
+        <v>2005</v>
       </c>
       <c r="C1142" s="2" t="s">
         <v>1701</v>
@@ -27349,7 +27433,7 @@
         <v>941</v>
       </c>
       <c r="E1171" s="2" t="s">
-        <v>1977</v>
+        <v>1972</v>
       </c>
       <c r="K1171" s="27"/>
     </row>
@@ -27412,14 +27496,14 @@
         <v>941</v>
       </c>
       <c r="E1175" s="2" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="F1175" s="2" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="K1175" s="27"/>
       <c r="M1175" s="5" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="1176" spans="1:14" x14ac:dyDescent="0.3">
@@ -27436,11 +27520,11 @@
         <v>941</v>
       </c>
       <c r="E1176" s="2" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="K1176" s="27"/>
       <c r="M1176" s="5" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="1177" spans="1:14" x14ac:dyDescent="0.3">
@@ -27562,20 +27646,20 @@
         <v>941</v>
       </c>
       <c r="E1184" s="4" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="F1184" s="2" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="G1184" s="2">
         <v>61</v>
       </c>
       <c r="K1184" s="27"/>
       <c r="M1184" s="5" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="N1184" s="25" t="s">
-        <v>2007</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="1185" spans="1:13" x14ac:dyDescent="0.3">
@@ -27622,7 +27706,7 @@
         <v>941</v>
       </c>
       <c r="E1187" s="2" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="K1187" s="27"/>
     </row>
@@ -27700,11 +27784,11 @@
         <v>941</v>
       </c>
       <c r="E1192" s="2" t="s">
-        <v>2057</v>
+        <v>2049</v>
       </c>
       <c r="K1192" s="27"/>
       <c r="M1192" s="5" t="s">
-        <v>2058</v>
+        <v>2050</v>
       </c>
     </row>
     <row r="1193" spans="1:13" x14ac:dyDescent="0.3">
@@ -27811,7 +27895,7 @@
         <v>941</v>
       </c>
       <c r="E1199" s="2" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="K1199" s="27"/>
     </row>
@@ -27845,7 +27929,7 @@
       </c>
       <c r="K1201" s="27"/>
       <c r="M1201" s="5" t="s">
-        <v>2009</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="1202" spans="1:13" x14ac:dyDescent="0.3">
@@ -27877,7 +27961,7 @@
         <v>941</v>
       </c>
       <c r="E1203" s="2" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="K1203" s="27"/>
     </row>
@@ -27970,7 +28054,7 @@
         <v>941</v>
       </c>
       <c r="E1209" s="2" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="K1209" s="27"/>
     </row>
@@ -28528,7 +28612,7 @@
         <v>941</v>
       </c>
       <c r="E1246" s="2" t="s">
-        <v>1972</v>
+        <v>1967</v>
       </c>
       <c r="K1246" s="27"/>
     </row>
@@ -28771,11 +28855,11 @@
         <v>941</v>
       </c>
       <c r="E1262" s="4" t="s">
-        <v>1920</v>
+        <v>1918</v>
       </c>
       <c r="K1262" s="27"/>
       <c r="M1262" s="5" t="s">
-        <v>1922</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="1263" spans="1:13" x14ac:dyDescent="0.3">
@@ -28837,7 +28921,7 @@
         <v>941</v>
       </c>
       <c r="E1266" s="2" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="K1266" s="27"/>
     </row>
@@ -28870,7 +28954,7 @@
         <v>941</v>
       </c>
       <c r="E1268" s="2" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="K1268" s="27"/>
     </row>
@@ -28948,11 +29032,11 @@
         <v>941</v>
       </c>
       <c r="E1273" s="2" t="s">
-        <v>2004</v>
+        <v>1998</v>
       </c>
       <c r="K1273" s="27"/>
       <c r="M1273" s="5" t="s">
-        <v>2077</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="1274" spans="1:13" x14ac:dyDescent="0.3">
@@ -29149,10 +29233,10 @@
         <v>941</v>
       </c>
       <c r="E1286" s="4" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="F1286" s="2" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="G1286" s="2">
         <v>25</v>
@@ -29224,14 +29308,14 @@
         <v>941</v>
       </c>
       <c r="E1290" s="2" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="G1290" s="2">
         <v>80</v>
       </c>
       <c r="K1290" s="27"/>
       <c r="M1290" s="5" t="s">
-        <v>1941</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="1291" spans="1:13" ht="30" x14ac:dyDescent="0.3">
@@ -29248,11 +29332,11 @@
         <v>941</v>
       </c>
       <c r="E1291" s="2" t="s">
-        <v>1915</v>
+        <v>1913</v>
       </c>
       <c r="K1291" s="27"/>
       <c r="M1291" s="5" t="s">
-        <v>1916</v>
+        <v>1914</v>
       </c>
     </row>
     <row r="1292" spans="1:13" x14ac:dyDescent="0.3">
@@ -29314,11 +29398,11 @@
         <v>941</v>
       </c>
       <c r="E1295" s="2" t="s">
-        <v>1997</v>
+        <v>1991</v>
       </c>
       <c r="K1295" s="27"/>
       <c r="M1295" s="5" t="s">
-        <v>1999</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="1296" spans="1:13" x14ac:dyDescent="0.3">
@@ -29410,11 +29494,11 @@
         <v>941</v>
       </c>
       <c r="E1301" s="2" t="s">
-        <v>1955</v>
+        <v>1951</v>
       </c>
       <c r="K1301" s="27"/>
       <c r="M1301" s="5" t="s">
-        <v>1956</v>
+        <v>1952</v>
       </c>
     </row>
     <row r="1302" spans="1:13" x14ac:dyDescent="0.3">
@@ -29551,7 +29635,7 @@
         <v>941</v>
       </c>
       <c r="E1310" s="2" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="K1310" s="27"/>
     </row>
@@ -29669,7 +29753,7 @@
       </c>
       <c r="K1317" s="27"/>
       <c r="M1317" s="5" t="s">
-        <v>2107</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="1318" spans="1:13" x14ac:dyDescent="0.3">
@@ -29950,7 +30034,7 @@
         <v>1819</v>
       </c>
       <c r="F1335" s="2" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="G1335" s="2">
         <v>38</v>
@@ -29960,7 +30044,7 @@
       </c>
       <c r="K1335" s="27"/>
       <c r="M1335" s="5" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="1336" spans="1:13" x14ac:dyDescent="0.3">
@@ -30136,7 +30220,7 @@
         <v>3.5</v>
       </c>
       <c r="M1346" s="5" t="s">
-        <v>2128</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="1347" spans="1:13" x14ac:dyDescent="0.3">
@@ -30231,14 +30315,14 @@
         <v>1806</v>
       </c>
       <c r="F1352" s="2" t="s">
-        <v>2096</v>
+        <v>1900</v>
       </c>
       <c r="G1352" s="2">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="K1352" s="27"/>
       <c r="M1352" s="5" t="s">
-        <v>2010</v>
+        <v>2174</v>
       </c>
     </row>
     <row r="1353" spans="1:13" x14ac:dyDescent="0.3">
@@ -30364,7 +30448,7 @@
       </c>
       <c r="K1360" s="27"/>
       <c r="M1360" s="5" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="1361" spans="1:13" x14ac:dyDescent="0.3">
@@ -30436,7 +30520,7 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="1365" spans="1:13" ht="30" x14ac:dyDescent="0.3">
+    <row r="1365" spans="1:13" ht="45" x14ac:dyDescent="0.3">
       <c r="A1365" s="3">
         <v>5443</v>
       </c>
@@ -30450,17 +30534,17 @@
         <v>941</v>
       </c>
       <c r="E1365" s="4" t="s">
-        <v>1930</v>
+        <v>1928</v>
       </c>
       <c r="F1365" s="2" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="G1365" s="2">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="K1365" s="27"/>
       <c r="M1365" s="5" t="s">
-        <v>1931</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="1366" spans="1:13" x14ac:dyDescent="0.3">
@@ -30502,7 +30586,7 @@
       </c>
       <c r="K1367" s="27"/>
       <c r="M1367" s="5" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="1368" spans="1:13" x14ac:dyDescent="0.3">
@@ -30682,7 +30766,7 @@
       </c>
       <c r="K1378" s="27"/>
       <c r="M1378" s="5" t="s">
-        <v>1925</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="1379" spans="1:13" x14ac:dyDescent="0.3">
@@ -30700,7 +30784,7 @@
       </c>
       <c r="K1379" s="27"/>
       <c r="M1379" s="5" t="s">
-        <v>1926</v>
+        <v>1924</v>
       </c>
     </row>
     <row r="1380" spans="1:13" x14ac:dyDescent="0.3">
@@ -30777,7 +30861,7 @@
         <v>941</v>
       </c>
       <c r="E1384" s="2" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="G1384" s="2">
         <v>12</v>
@@ -31008,10 +31092,10 @@
         <v>941</v>
       </c>
       <c r="E1399" s="2" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="F1399" s="2" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="G1399" s="2">
         <v>50</v>
@@ -31162,7 +31246,7 @@
       </c>
       <c r="K1408" s="27"/>
       <c r="M1408" s="5" t="s">
-        <v>2017</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="1409" spans="1:13" x14ac:dyDescent="0.3">
@@ -31518,14 +31602,14 @@
         <v>941</v>
       </c>
       <c r="E1431" s="4" t="s">
-        <v>1936</v>
+        <v>1933</v>
       </c>
       <c r="F1431" s="2" t="s">
         <v>1810</v>
       </c>
       <c r="K1431" s="27"/>
       <c r="M1431" s="5" t="s">
-        <v>1937</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="1432" spans="1:13" x14ac:dyDescent="0.3">
@@ -31572,7 +31656,7 @@
         <v>941</v>
       </c>
       <c r="E1434" s="4" t="s">
-        <v>1917</v>
+        <v>1915</v>
       </c>
       <c r="K1434" s="27"/>
     </row>
@@ -31650,10 +31734,10 @@
         <v>941</v>
       </c>
       <c r="E1439" s="2" t="s">
-        <v>1965</v>
+        <v>1961</v>
       </c>
       <c r="F1439" s="2" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="G1439" s="2">
         <v>72</v>
@@ -31879,7 +31963,7 @@
       </c>
       <c r="K1453" s="27"/>
       <c r="M1453" s="5" t="s">
-        <v>2035</v>
+        <v>2027</v>
       </c>
     </row>
     <row r="1454" spans="1:13" x14ac:dyDescent="0.3">
@@ -32243,11 +32327,17 @@
       <c r="D1476" s="2" t="s">
         <v>941</v>
       </c>
+      <c r="E1476" s="2" t="s">
+        <v>1853</v>
+      </c>
+      <c r="G1476" s="2">
+        <v>19</v>
+      </c>
       <c r="K1476" s="27" t="s">
-        <v>2137</v>
+        <v>2125</v>
       </c>
       <c r="M1476" s="5" t="s">
-        <v>2079</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="1477" spans="1:13" x14ac:dyDescent="0.3">
@@ -32279,7 +32369,7 @@
         <v>941</v>
       </c>
       <c r="E1478" s="2" t="s">
-        <v>1918</v>
+        <v>1916</v>
       </c>
       <c r="K1478" s="27"/>
     </row>
@@ -32312,7 +32402,7 @@
         <v>941</v>
       </c>
       <c r="E1480" s="4" t="s">
-        <v>1938</v>
+        <v>1935</v>
       </c>
       <c r="F1480" s="2" t="s">
         <v>1820</v>
@@ -32322,7 +32412,7 @@
       </c>
       <c r="K1480" s="27"/>
       <c r="M1480" s="5" t="s">
-        <v>1939</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="1481" spans="1:13" x14ac:dyDescent="0.3">
@@ -32747,14 +32837,14 @@
         <v>1803</v>
       </c>
       <c r="F1507" s="2" t="s">
-        <v>2093</v>
+        <v>2085</v>
       </c>
       <c r="G1507" s="2">
         <v>70</v>
       </c>
       <c r="K1507" s="27"/>
       <c r="M1507" s="5" t="s">
-        <v>2097</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="1508" spans="1:13" x14ac:dyDescent="0.3">
@@ -32861,11 +32951,11 @@
         <v>941</v>
       </c>
       <c r="E1514" s="2" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="K1514" s="27"/>
       <c r="M1514" s="5" t="s">
-        <v>1934</v>
+        <v>1931</v>
       </c>
     </row>
     <row r="1515" spans="1:13" x14ac:dyDescent="0.3">
@@ -33005,17 +33095,19 @@
         <v>941</v>
       </c>
       <c r="E1523" s="4" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="F1523" s="2" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="G1523" s="2">
         <v>120</v>
       </c>
-      <c r="K1523" s="27"/>
+      <c r="K1523" s="27" t="s">
+        <v>2176</v>
+      </c>
       <c r="M1523" s="5" t="s">
-        <v>1842</v>
+        <v>2177</v>
       </c>
     </row>
     <row r="1524" spans="1:13" x14ac:dyDescent="0.3">
@@ -33032,7 +33124,7 @@
         <v>941</v>
       </c>
       <c r="E1524" s="2" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="K1524" s="27"/>
     </row>
@@ -33204,7 +33296,7 @@
       </c>
       <c r="K1535" s="27"/>
       <c r="M1535" s="5" t="s">
-        <v>1949</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="1536" spans="1:13" x14ac:dyDescent="0.3">
@@ -33266,11 +33358,11 @@
         <v>941</v>
       </c>
       <c r="E1539" s="4" t="s">
-        <v>1920</v>
+        <v>1918</v>
       </c>
       <c r="K1539" s="27"/>
       <c r="M1539" s="5" t="s">
-        <v>1924</v>
+        <v>1922</v>
       </c>
     </row>
     <row r="1540" spans="1:13" x14ac:dyDescent="0.3">
@@ -33335,11 +33427,11 @@
         <v>941</v>
       </c>
       <c r="E1543" s="2" t="s">
-        <v>1985</v>
+        <v>1979</v>
       </c>
       <c r="K1543" s="27"/>
       <c r="M1543" s="5" t="s">
-        <v>2083</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="1544" spans="1:13" x14ac:dyDescent="0.3">
@@ -33461,11 +33553,11 @@
         <v>941</v>
       </c>
       <c r="E1551" s="4" t="s">
-        <v>1920</v>
+        <v>1918</v>
       </c>
       <c r="K1551" s="27"/>
       <c r="M1551" s="5" t="s">
-        <v>1923</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="1552" spans="1:13" x14ac:dyDescent="0.3">
@@ -33593,10 +33685,10 @@
         <v>941</v>
       </c>
       <c r="K1558" s="27" t="s">
-        <v>2138</v>
+        <v>2126</v>
       </c>
       <c r="M1558" s="5" t="s">
-        <v>2139</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="1559" spans="1:13" x14ac:dyDescent="0.3">
@@ -33627,7 +33719,15 @@
       <c r="D1560" s="2" t="s">
         <v>941</v>
       </c>
-      <c r="K1560" s="27"/>
+      <c r="E1560" s="2" t="s">
+        <v>2180</v>
+      </c>
+      <c r="K1560" s="27" t="s">
+        <v>2182</v>
+      </c>
+      <c r="M1560" s="5" t="s">
+        <v>2181</v>
+      </c>
     </row>
     <row r="1561" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1561" s="3">
@@ -33673,7 +33773,7 @@
         <v>941</v>
       </c>
       <c r="E1563" s="2" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="K1563" s="27"/>
     </row>
@@ -33736,7 +33836,7 @@
         <v>941</v>
       </c>
       <c r="E1567" s="2" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="K1567" s="27"/>
     </row>
@@ -33937,11 +34037,11 @@
         <v>941</v>
       </c>
       <c r="E1580" s="4" t="s">
-        <v>1962</v>
+        <v>1958</v>
       </c>
       <c r="K1580" s="27"/>
       <c r="M1580" s="5" t="s">
-        <v>1961</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="1581" spans="1:13" x14ac:dyDescent="0.3">
@@ -34099,14 +34199,14 @@
         <v>1824</v>
       </c>
       <c r="F1590" s="2" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="G1590" s="2">
         <v>103</v>
       </c>
       <c r="K1590" s="27"/>
       <c r="M1590" s="5" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="1591" spans="1:13" x14ac:dyDescent="0.3">
@@ -34228,7 +34328,7 @@
         <v>941</v>
       </c>
       <c r="E1598" s="4" t="s">
-        <v>2098</v>
+        <v>2089</v>
       </c>
       <c r="G1598" s="2">
         <v>81</v>
@@ -34313,7 +34413,7 @@
       </c>
       <c r="K1603" s="27"/>
       <c r="M1603" s="5" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="1604" spans="1:13" x14ac:dyDescent="0.3">
@@ -34349,7 +34449,7 @@
       </c>
       <c r="K1605" s="27"/>
       <c r="M1605" s="5" t="s">
-        <v>2113</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="1606" spans="1:13" x14ac:dyDescent="0.3">
@@ -34410,6 +34510,9 @@
       <c r="D1609" s="2" t="s">
         <v>941</v>
       </c>
+      <c r="E1609" s="2" t="s">
+        <v>2180</v>
+      </c>
       <c r="K1609" s="27"/>
     </row>
     <row r="1610" spans="1:13" x14ac:dyDescent="0.3">
@@ -34516,7 +34619,7 @@
         <v>941</v>
       </c>
       <c r="E1616" s="2" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="F1616" s="2" t="s">
         <v>1767</v>
@@ -34526,7 +34629,7 @@
       </c>
       <c r="K1616" s="27"/>
       <c r="M1616" s="5" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="1617" spans="1:11" x14ac:dyDescent="0.3">
@@ -34666,7 +34769,7 @@
         <v>941</v>
       </c>
       <c r="E1625" s="2" t="s">
-        <v>1950</v>
+        <v>1946</v>
       </c>
       <c r="K1625" s="27"/>
     </row>
@@ -34948,17 +35051,17 @@
         <v>941</v>
       </c>
       <c r="E1643" s="4" t="s">
-        <v>1952</v>
+        <v>1948</v>
       </c>
       <c r="F1643" s="4" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="G1643" s="2">
         <v>25</v>
       </c>
       <c r="K1643" s="27"/>
       <c r="M1643" s="5" t="s">
-        <v>2105</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="1644" spans="1:13" x14ac:dyDescent="0.3">
@@ -35009,7 +35112,7 @@
       </c>
       <c r="K1646" s="27"/>
       <c r="M1646" s="5" t="s">
-        <v>1951</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="1647" spans="1:13" x14ac:dyDescent="0.3">
@@ -35101,14 +35204,14 @@
         <v>941</v>
       </c>
       <c r="E1652" s="2" t="s">
-        <v>2121</v>
+        <v>2111</v>
       </c>
       <c r="G1652" s="2">
         <v>451</v>
       </c>
       <c r="K1652" s="27"/>
       <c r="M1652" s="5" t="s">
-        <v>2122</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="1653" spans="1:13" x14ac:dyDescent="0.3">
@@ -35125,13 +35228,19 @@
         <v>941</v>
       </c>
       <c r="E1653" s="2" t="s">
-        <v>2143</v>
+        <v>2131</v>
+      </c>
+      <c r="F1653" s="2" t="s">
+        <v>2178</v>
+      </c>
+      <c r="G1653" s="2">
+        <v>55</v>
       </c>
       <c r="K1653" s="27" t="s">
-        <v>2144</v>
+        <v>2132</v>
       </c>
       <c r="M1653" s="5" t="s">
-        <v>2145</v>
+        <v>2133</v>
       </c>
     </row>
     <row r="1654" spans="1:13" x14ac:dyDescent="0.3">
@@ -35178,7 +35287,7 @@
         <v>941</v>
       </c>
       <c r="E1656" s="2" t="s">
-        <v>2008</v>
+        <v>2002</v>
       </c>
       <c r="K1656" s="27"/>
     </row>
@@ -35754,19 +35863,19 @@
         <v>941</v>
       </c>
       <c r="E1694" s="2" t="s">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="F1694" s="2" t="s">
-        <v>2014</v>
+        <v>1900</v>
       </c>
       <c r="G1694" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K1694" s="27" t="s">
-        <v>2141</v>
+        <v>2129</v>
       </c>
       <c r="M1694" s="5" t="s">
-        <v>2140</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="1695" spans="1:13" x14ac:dyDescent="0.3">
@@ -35936,7 +36045,7 @@
         <v>941</v>
       </c>
       <c r="E1705" s="2" t="s">
-        <v>2116</v>
+        <v>2106</v>
       </c>
       <c r="G1705" s="2">
         <v>48</v>
@@ -36332,7 +36441,7 @@
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="D2" s="2" t="s">
-        <v>1991</v>
+        <v>1985</v>
       </c>
       <c r="E2" s="2">
         <v>15877</v>
@@ -36340,22 +36449,22 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>1992</v>
+        <v>1986</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>1993</v>
+        <v>1987</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>1994</v>
+        <v>1988</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>1995</v>
+        <v>1989</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>1996</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update 2020 sd information
</commit_message>
<xml_diff>
--- a/all_stock.xlsx
+++ b/all_stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\download\rich_stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4855F44E-881F-4630-9E79-8FE138C62708}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C2AC3F-EF71-40C9-B20E-87F12F146906}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5932" uniqueCount="2204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5933" uniqueCount="2205">
   <si>
     <t>代碼</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -7366,6 +7366,10 @@
   </si>
   <si>
     <t>[2020 EPS] 2.95</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>定存股</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7920,8 +7924,8 @@
   <dimension ref="A1:N1713"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1645" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1653" sqref="I1653"/>
+      <pane ySplit="1" topLeftCell="A285" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G292" sqref="G292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -8529,11 +8533,11 @@
       <c r="D32" s="2" t="s">
         <v>940</v>
       </c>
+      <c r="F32" s="2" t="s">
+        <v>2204</v>
+      </c>
       <c r="G32" s="2">
         <v>31</v>
-      </c>
-      <c r="I32" s="2">
-        <v>33.1</v>
       </c>
       <c r="K32" s="27" t="s">
         <v>2201</v>
@@ -12814,6 +12818,9 @@
       <c r="F291" s="2" t="s">
         <v>2191</v>
       </c>
+      <c r="G291" s="2">
+        <v>310</v>
+      </c>
       <c r="K291" s="27"/>
     </row>
     <row r="292" spans="1:13" ht="30" x14ac:dyDescent="0.3">
@@ -25968,10 +25975,7 @@
         <v>2193</v>
       </c>
       <c r="G1072" s="2">
-        <v>750</v>
-      </c>
-      <c r="I1072" s="2">
-        <v>752</v>
+        <v>720</v>
       </c>
       <c r="K1072" s="27" t="s">
         <v>2127</v>
@@ -35342,10 +35346,10 @@
         <v>2108</v>
       </c>
       <c r="G1652" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I1652" s="2">
-        <v>450</v>
+        <v>470</v>
       </c>
       <c r="K1652" s="27"/>
       <c r="M1652" s="5" t="s">

</xml_diff>

<commit_message>
update 2021/03 and news
</commit_message>
<xml_diff>
--- a/all_stock.xlsx
+++ b/all_stock.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\download\rich_stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2910001-B1BD-4F49-A249-699850CF9404}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A7B6FE-E855-4289-86D3-C85663509410}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5839" uniqueCount="2116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5838" uniqueCount="2115">
   <si>
     <t>代碼</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6671,17 +6671,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>華義列警示股 10月每股虧損0.13元
-12月自結稅後純益1,100萬元，每股純益0.81元，</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>核心
-短期注意</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>衛星
 短期注意</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6961,6 +6951,10 @@
   </si>
   <si>
     <t>核心</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020/12月自結稅後純益1,100萬元，每股純益0.81元，</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7515,8 +7509,8 @@
   <dimension ref="A1:N1711"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A494" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A502" sqref="A502:XFD502"/>
+      <pane ySplit="1" topLeftCell="A273" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I281" sqref="I281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -7569,7 +7563,7 @@
         <v>1712</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>2066</v>
+        <v>2064</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>1971</v>
@@ -7605,7 +7599,7 @@
       </c>
       <c r="K2" s="27"/>
       <c r="M2" s="5" t="s">
-        <v>2063</v>
+        <v>2061</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -7622,7 +7616,7 @@
         <v>939</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>2064</v>
+        <v>2062</v>
       </c>
       <c r="G3" s="2">
         <v>41</v>
@@ -8039,7 +8033,7 @@
         <v>939</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>2061</v>
+        <v>2059</v>
       </c>
       <c r="K27" s="27"/>
     </row>
@@ -8120,7 +8114,7 @@
         <v>939</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>2062</v>
+        <v>2060</v>
       </c>
       <c r="G32" s="2">
         <v>31</v>
@@ -8309,7 +8303,7 @@
       </c>
       <c r="K44" s="27"/>
       <c r="M44" s="5" t="s">
-        <v>2067</v>
+        <v>2065</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
@@ -9330,7 +9324,7 @@
       <c r="K107" s="27"/>
       <c r="L107" s="4"/>
       <c r="M107" s="5" t="s">
-        <v>2068</v>
+        <v>2066</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.3">
@@ -11660,14 +11654,14 @@
         <v>1795</v>
       </c>
       <c r="F251" s="4" t="s">
-        <v>2110</v>
+        <v>2108</v>
       </c>
       <c r="G251" s="2">
         <v>100</v>
       </c>
       <c r="K251" s="27"/>
       <c r="M251" s="5" t="s">
-        <v>2111</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="252" spans="1:13" x14ac:dyDescent="0.3">
@@ -11849,7 +11843,7 @@
       </c>
       <c r="K261" s="27"/>
       <c r="M261" s="5" t="s">
-        <v>2069</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="262" spans="1:13" x14ac:dyDescent="0.3">
@@ -11989,10 +11983,7 @@
         <v>939</v>
       </c>
       <c r="E269" s="2" t="s">
-        <v>2114</v>
-      </c>
-      <c r="I269" s="2">
-        <v>27.3</v>
+        <v>2112</v>
       </c>
       <c r="K269" s="27"/>
     </row>
@@ -12013,7 +12004,7 @@
         <v>1764</v>
       </c>
       <c r="F270" s="2" t="s">
-        <v>2112</v>
+        <v>2110</v>
       </c>
       <c r="G270" s="2">
         <v>420</v>
@@ -12201,6 +12192,9 @@
       <c r="F280" s="2" t="s">
         <v>1897</v>
       </c>
+      <c r="I280" s="2">
+        <v>35.200000000000003</v>
+      </c>
       <c r="K280" s="27"/>
     </row>
     <row r="281" spans="1:13" x14ac:dyDescent="0.3">
@@ -12422,7 +12416,7 @@
       </c>
       <c r="K292" s="27"/>
       <c r="M292" s="5" t="s">
-        <v>2070</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="293" spans="1:13" x14ac:dyDescent="0.3">
@@ -12650,7 +12644,7 @@
       </c>
       <c r="K305" s="27"/>
       <c r="M305" s="5" t="s">
-        <v>2071</v>
+        <v>2069</v>
       </c>
     </row>
     <row r="306" spans="1:13" x14ac:dyDescent="0.3">
@@ -12722,7 +12716,7 @@
       </c>
       <c r="K308" s="27"/>
       <c r="M308" s="5" t="s">
-        <v>2072</v>
+        <v>2070</v>
       </c>
     </row>
     <row r="309" spans="1:13" x14ac:dyDescent="0.3">
@@ -12754,7 +12748,7 @@
         <v>939</v>
       </c>
       <c r="E310" s="2" t="s">
-        <v>2113</v>
+        <v>2111</v>
       </c>
       <c r="F310" s="2" t="s">
         <v>1897</v>
@@ -12787,7 +12781,7 @@
         <v>7</v>
       </c>
       <c r="M311" s="5" t="s">
-        <v>2073</v>
+        <v>2071</v>
       </c>
     </row>
     <row r="312" spans="1:13" x14ac:dyDescent="0.3">
@@ -13147,7 +13141,7 @@
       </c>
       <c r="K332" s="27"/>
       <c r="M332" s="5" t="s">
-        <v>2074</v>
+        <v>2072</v>
       </c>
     </row>
     <row r="333" spans="1:13" x14ac:dyDescent="0.3">
@@ -13390,7 +13384,7 @@
       </c>
       <c r="K347" s="27"/>
       <c r="M347" s="5" t="s">
-        <v>2075</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="348" spans="1:13" x14ac:dyDescent="0.3">
@@ -13672,7 +13666,7 @@
       </c>
       <c r="K363" s="27"/>
       <c r="M363" s="5" t="s">
-        <v>2076</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="364" spans="1:13" x14ac:dyDescent="0.3">
@@ -15196,7 +15190,7 @@
       </c>
       <c r="K459" s="27"/>
       <c r="M459" s="5" t="s">
-        <v>2077</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="460" spans="1:13" x14ac:dyDescent="0.3">
@@ -15508,7 +15502,7 @@
       </c>
       <c r="K478" s="27"/>
       <c r="M478" s="5" t="s">
-        <v>2078</v>
+        <v>2076</v>
       </c>
     </row>
     <row r="479" spans="1:13" x14ac:dyDescent="0.3">
@@ -15550,7 +15544,7 @@
       </c>
       <c r="K480" s="27"/>
       <c r="M480" s="5" t="s">
-        <v>2079</v>
+        <v>2077</v>
       </c>
     </row>
     <row r="481" spans="1:13" x14ac:dyDescent="0.3">
@@ -15577,7 +15571,7 @@
       </c>
       <c r="K481" s="27"/>
       <c r="M481" s="5" t="s">
-        <v>2080</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="482" spans="1:13" x14ac:dyDescent="0.3">
@@ -16003,7 +15997,7 @@
       </c>
       <c r="K507" s="27"/>
       <c r="M507" s="5" t="s">
-        <v>2081</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="508" spans="1:13" x14ac:dyDescent="0.3">
@@ -16436,7 +16430,7 @@
       </c>
       <c r="K532" s="27"/>
       <c r="M532" s="5" t="s">
-        <v>2082</v>
+        <v>2080</v>
       </c>
     </row>
     <row r="533" spans="1:13" x14ac:dyDescent="0.3">
@@ -17924,7 +17918,7 @@
       </c>
       <c r="K622" s="27"/>
       <c r="M622" s="5" t="s">
-        <v>2083</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="623" spans="1:13" x14ac:dyDescent="0.3">
@@ -18377,7 +18371,7 @@
       </c>
       <c r="K648" s="27"/>
       <c r="M648" s="5" t="s">
-        <v>2084</v>
+        <v>2082</v>
       </c>
     </row>
     <row r="649" spans="1:13" x14ac:dyDescent="0.3">
@@ -18665,7 +18659,7 @@
       </c>
       <c r="K666" s="27"/>
       <c r="M666" s="5" t="s">
-        <v>2085</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="667" spans="1:13" x14ac:dyDescent="0.3">
@@ -18983,7 +18977,7 @@
       </c>
       <c r="K685" s="27"/>
       <c r="M685" s="5" t="s">
-        <v>2086</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="686" spans="1:13" x14ac:dyDescent="0.3">
@@ -19295,7 +19289,7 @@
       </c>
       <c r="K703" s="27"/>
       <c r="M703" s="5" t="s">
-        <v>2087</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="704" spans="1:13" x14ac:dyDescent="0.3">
@@ -19553,7 +19547,7 @@
       </c>
       <c r="K718" s="27"/>
       <c r="M718" s="5" t="s">
-        <v>2088</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="719" spans="1:13" x14ac:dyDescent="0.3">
@@ -19793,7 +19787,7 @@
       </c>
       <c r="K733" s="27"/>
       <c r="M733" s="5" t="s">
-        <v>2089</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="734" spans="1:13" x14ac:dyDescent="0.3">
@@ -19925,7 +19919,7 @@
       </c>
       <c r="K741" s="27"/>
       <c r="M741" s="5" t="s">
-        <v>2090</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="742" spans="1:13" x14ac:dyDescent="0.3">
@@ -20123,7 +20117,7 @@
       </c>
       <c r="K753" s="27"/>
       <c r="M753" s="5" t="s">
-        <v>2091</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="754" spans="1:13" x14ac:dyDescent="0.3">
@@ -20390,7 +20384,7 @@
       </c>
       <c r="K769" s="27"/>
       <c r="M769" s="5" t="s">
-        <v>2092</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="770" spans="1:13" ht="60" x14ac:dyDescent="0.3">
@@ -21196,11 +21190,11 @@
         <v>939</v>
       </c>
       <c r="E817" s="2" t="s">
-        <v>2058</v>
+        <v>2056</v>
       </c>
       <c r="K817" s="27"/>
       <c r="M817" s="5" t="s">
-        <v>2059</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="818" spans="1:13" x14ac:dyDescent="0.3">
@@ -21208,7 +21202,7 @@
         <v>6558</v>
       </c>
       <c r="B818" s="1" t="s">
-        <v>2060</v>
+        <v>2058</v>
       </c>
       <c r="C818" s="2" t="s">
         <v>3</v>
@@ -21641,7 +21635,7 @@
       </c>
       <c r="K843" s="27"/>
       <c r="M843" s="26" t="s">
-        <v>2093</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="844" spans="1:13" x14ac:dyDescent="0.3">
@@ -22229,7 +22223,7 @@
       </c>
       <c r="K879" s="27"/>
       <c r="M879" s="5" t="s">
-        <v>2094</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="880" spans="1:13" x14ac:dyDescent="0.3">
@@ -23120,7 +23114,7 @@
       </c>
       <c r="K935" s="27"/>
       <c r="M935" s="5" t="s">
-        <v>2095</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="936" spans="1:13" x14ac:dyDescent="0.3">
@@ -23216,7 +23210,7 @@
       </c>
       <c r="K940" s="27"/>
       <c r="M940" s="5" t="s">
-        <v>2096</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="941" spans="1:13" x14ac:dyDescent="0.3">
@@ -23300,7 +23294,7 @@
       </c>
       <c r="K945" s="27"/>
       <c r="M945" s="5" t="s">
-        <v>2097</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="946" spans="1:13" x14ac:dyDescent="0.3">
@@ -23852,7 +23846,7 @@
       </c>
       <c r="K978" s="27"/>
       <c r="M978" s="5" t="s">
-        <v>2098</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="979" spans="1:13" x14ac:dyDescent="0.3">
@@ -24413,7 +24407,7 @@
       </c>
       <c r="K1014" s="27"/>
     </row>
-    <row r="1015" spans="1:13" ht="30" x14ac:dyDescent="0.3">
+    <row r="1015" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1015" s="3">
         <v>3086</v>
       </c>
@@ -24434,7 +24428,7 @@
       </c>
       <c r="K1015" s="27"/>
       <c r="M1015" s="5" t="s">
-        <v>2055</v>
+        <v>2114</v>
       </c>
     </row>
     <row r="1016" spans="1:13" x14ac:dyDescent="0.3">
@@ -25345,14 +25339,17 @@
         <v>1776</v>
       </c>
       <c r="F1071" s="4" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="G1071" s="2">
         <v>720</v>
       </c>
+      <c r="I1071" s="2">
+        <v>790</v>
+      </c>
       <c r="K1071" s="27"/>
       <c r="M1071" s="7" t="s">
-        <v>2099</v>
+        <v>2097</v>
       </c>
       <c r="N1071" s="25" t="s">
         <v>1985</v>
@@ -25493,7 +25490,7 @@
       </c>
       <c r="K1080" s="27"/>
     </row>
-    <row r="1081" spans="1:13" ht="30" x14ac:dyDescent="0.3">
+    <row r="1081" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1081" s="3">
         <v>3324</v>
       </c>
@@ -25509,14 +25506,9 @@
       <c r="E1081" s="2" t="s">
         <v>1709</v>
       </c>
-      <c r="F1081" s="4" t="s">
-        <v>2057</v>
-      </c>
+      <c r="F1081" s="4"/>
       <c r="G1081" s="2">
         <v>144</v>
-      </c>
-      <c r="I1081" s="2">
-        <v>225</v>
       </c>
       <c r="K1081" s="27"/>
     </row>
@@ -26156,7 +26148,7 @@
       </c>
       <c r="K1121" s="27"/>
       <c r="M1121" s="5" t="s">
-        <v>2100</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="1122" spans="1:13" x14ac:dyDescent="0.3">
@@ -28523,7 +28515,7 @@
       </c>
       <c r="K1271" s="27"/>
       <c r="M1271" s="5" t="s">
-        <v>2101</v>
+        <v>2099</v>
       </c>
     </row>
     <row r="1272" spans="1:13" x14ac:dyDescent="0.3">
@@ -28889,7 +28881,7 @@
       </c>
       <c r="K1293" s="27"/>
       <c r="M1293" s="5" t="s">
-        <v>2102</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="1294" spans="1:13" x14ac:dyDescent="0.3">
@@ -29240,7 +29232,7 @@
       </c>
       <c r="K1315" s="27"/>
       <c r="M1315" s="5" t="s">
-        <v>2103</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="1316" spans="1:13" x14ac:dyDescent="0.3">
@@ -29531,7 +29523,7 @@
       </c>
       <c r="K1333" s="27"/>
       <c r="M1333" s="5" t="s">
-        <v>2065</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="1334" spans="1:13" x14ac:dyDescent="0.3">
@@ -32009,7 +32001,7 @@
       </c>
       <c r="K1486" s="27"/>
       <c r="M1486" s="5" t="s">
-        <v>2104</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="1487" spans="1:13" x14ac:dyDescent="0.3">
@@ -32306,7 +32298,7 @@
       </c>
       <c r="K1505" s="27"/>
       <c r="M1505" s="5" t="s">
-        <v>2105</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="1506" spans="1:13" x14ac:dyDescent="0.3">
@@ -32567,7 +32559,7 @@
       </c>
       <c r="K1521" s="27"/>
       <c r="M1521" s="5" t="s">
-        <v>2106</v>
+        <v>2104</v>
       </c>
     </row>
     <row r="1522" spans="1:13" x14ac:dyDescent="0.3">
@@ -33896,7 +33888,7 @@
       </c>
       <c r="K1603" s="27"/>
       <c r="M1603" s="5" t="s">
-        <v>2107</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="1604" spans="1:13" x14ac:dyDescent="0.3">
@@ -34654,14 +34646,14 @@
         <v>2025</v>
       </c>
       <c r="F1650" s="2" t="s">
-        <v>2115</v>
+        <v>2113</v>
       </c>
       <c r="G1650" s="2">
         <v>450</v>
       </c>
       <c r="K1650" s="27"/>
       <c r="M1650" s="5" t="s">
-        <v>2108</v>
+        <v>2106</v>
       </c>
     </row>
     <row r="1651" spans="1:13" x14ac:dyDescent="0.3">
@@ -35318,7 +35310,7 @@
       </c>
       <c r="K1692" s="27"/>
       <c r="M1692" s="5" t="s">
-        <v>2109</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="1693" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update tmp all information
</commit_message>
<xml_diff>
--- a/all_stock.xlsx
+++ b/all_stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\download\rich_stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD056E7-249C-42C6-8F82-AF27C8E5F259}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1093C76-BA70-4810-A997-E7D1DBDFDC7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5854" uniqueCount="2134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5852" uniqueCount="2128">
   <si>
     <t>代碼</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6857,29 +6857,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>核心
-短期注意</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>鋰電池</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>衛星
-短期注意</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>年年都配股</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>衛星
-短期注意</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>生醫股</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -6893,10 +6878,6 @@
   </si>
   <si>
     <t>國碳科主生產防火材料、防火塗料、防火工程、阻燃劑等，外銷比重約68％。國碳科持續推展北美、大陸及中東市場；占地約二千坪蘆竹廠辦合一新廠加入量產行列，搭配原有一廠生產支應未來三年接單成長。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>短期注意</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -6973,15 +6954,6 @@
   </si>
   <si>
     <t>Q1每股賺3.45元</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>衛星
-長期注意</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>短期注意</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -7610,8 +7582,8 @@
   <dimension ref="A1:M1697"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A278" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G286" sqref="G286"/>
+      <pane ySplit="1" topLeftCell="A1416" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1424" sqref="F1424"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -8215,16 +8187,16 @@
         <v>924</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>2130</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>2095</v>
+        <v>2124</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>2084</v>
       </c>
       <c r="I34" s="2">
         <v>29.5</v>
       </c>
       <c r="L34" s="5" t="s">
-        <v>2131</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -9475,16 +9447,16 @@
         <v>924</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>2107</v>
+        <v>2103</v>
       </c>
       <c r="F116" s="4" t="s">
-        <v>2109</v>
+        <v>2105</v>
       </c>
       <c r="L116" s="5" t="s">
-        <v>2108</v>
+        <v>2104</v>
       </c>
       <c r="M116" s="25" t="s">
-        <v>2106</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.3">
@@ -9650,16 +9622,16 @@
         <v>924</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>2116</v>
+        <v>2110</v>
       </c>
       <c r="F127" s="4" t="s">
-        <v>2118</v>
+        <v>2112</v>
       </c>
       <c r="G127" s="2">
         <v>140</v>
       </c>
       <c r="L127" s="5" t="s">
-        <v>2117</v>
+        <v>2111</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.3">
@@ -9732,7 +9704,7 @@
         <v>924</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>2119</v>
+        <v>2113</v>
       </c>
     </row>
     <row r="133" spans="1:12" x14ac:dyDescent="0.3">
@@ -10270,7 +10242,7 @@
         <v>1822</v>
       </c>
       <c r="F167" s="2" t="s">
-        <v>2102</v>
+        <v>2098</v>
       </c>
       <c r="G167" s="2">
         <v>36</v>
@@ -11119,7 +11091,7 @@
         <v>75</v>
       </c>
       <c r="L224" s="5" t="s">
-        <v>2132</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.3">
@@ -12002,16 +11974,16 @@
         <v>924</v>
       </c>
       <c r="E277" s="2" t="s">
-        <v>2125</v>
+        <v>2119</v>
       </c>
       <c r="F277" s="2" t="s">
-        <v>2126</v>
+        <v>2120</v>
       </c>
       <c r="G277" s="2">
         <v>70</v>
       </c>
       <c r="L277" s="5" t="s">
-        <v>2127</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.3">
@@ -13049,9 +13021,6 @@
       <c r="D339" s="2" t="s">
         <v>924</v>
       </c>
-      <c r="F339" s="2" t="s">
-        <v>2095</v>
-      </c>
     </row>
     <row r="340" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A340" s="3">
@@ -13386,7 +13355,7 @@
         <v>924</v>
       </c>
       <c r="E360" s="4" t="s">
-        <v>2100</v>
+        <v>2096</v>
       </c>
       <c r="F360" s="2" t="s">
         <v>2081</v>
@@ -13398,7 +13367,7 @@
         <v>121</v>
       </c>
       <c r="L360" s="5" t="s">
-        <v>2098</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="361" spans="1:12" x14ac:dyDescent="0.3">
@@ -13797,7 +13766,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="385" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A385" s="3">
         <v>2486</v>
       </c>
@@ -13814,7 +13783,7 @@
         <v>1835</v>
       </c>
       <c r="F385" s="4" t="s">
-        <v>2084</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="386" spans="1:7" x14ac:dyDescent="0.3">
@@ -13845,10 +13814,10 @@
         <v>924</v>
       </c>
       <c r="E387" s="2" t="s">
-        <v>2110</v>
+        <v>2106</v>
       </c>
       <c r="F387" s="2" t="s">
-        <v>2111</v>
+        <v>2107</v>
       </c>
     </row>
     <row r="388" spans="1:7" x14ac:dyDescent="0.3">
@@ -15941,16 +15910,16 @@
         <v>924</v>
       </c>
       <c r="E524" s="2" t="s">
-        <v>2112</v>
+        <v>2108</v>
       </c>
       <c r="F524" s="4" t="s">
-        <v>2114</v>
+        <v>2084</v>
       </c>
       <c r="G524" s="2">
         <v>130</v>
       </c>
       <c r="L524" s="5" t="s">
-        <v>2113</v>
+        <v>2109</v>
       </c>
     </row>
     <row r="525" spans="1:12" x14ac:dyDescent="0.3">
@@ -15969,9 +15938,6 @@
       <c r="E525" s="2" t="s">
         <v>1749</v>
       </c>
-      <c r="F525" s="2" t="s">
-        <v>2115</v>
-      </c>
     </row>
     <row r="526" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A526" s="3">
@@ -16131,7 +16097,7 @@
         <v>924</v>
       </c>
       <c r="E535" s="4" t="s">
-        <v>2101</v>
+        <v>2097</v>
       </c>
       <c r="F535" s="2" t="s">
         <v>1874</v>
@@ -16140,7 +16106,7 @@
         <v>95</v>
       </c>
       <c r="L535" s="5" t="s">
-        <v>2105</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="536" spans="1:12" x14ac:dyDescent="0.3">
@@ -16835,7 +16801,7 @@
         <v>1798</v>
       </c>
       <c r="F581" s="2" t="s">
-        <v>2097</v>
+        <v>2093</v>
       </c>
       <c r="I581" s="2">
         <v>552</v>
@@ -17493,7 +17459,7 @@
         <v>2039</v>
       </c>
     </row>
-    <row r="623" spans="1:12" ht="30" x14ac:dyDescent="0.3">
+    <row r="623" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A623" s="3">
         <v>3679</v>
       </c>
@@ -17510,7 +17476,7 @@
         <v>1981</v>
       </c>
       <c r="F623" s="4" t="s">
-        <v>2084</v>
+        <v>1855</v>
       </c>
       <c r="G623" s="2">
         <v>120</v>
@@ -20467,13 +20433,13 @@
         <v>1966</v>
       </c>
       <c r="F810" s="2" t="s">
-        <v>2103</v>
+        <v>2099</v>
       </c>
       <c r="G810" s="2">
         <v>266</v>
       </c>
       <c r="L810" s="5" t="s">
-        <v>2104</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="811" spans="1:12" x14ac:dyDescent="0.3">
@@ -21060,7 +21026,7 @@
         <v>924</v>
       </c>
       <c r="E847" s="4" t="s">
-        <v>2101</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="848" spans="1:12" x14ac:dyDescent="0.3">
@@ -23496,7 +23462,7 @@
         <v>924</v>
       </c>
       <c r="E1006" s="2" t="s">
-        <v>2099</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="1007" spans="1:12" x14ac:dyDescent="0.3">
@@ -23687,13 +23653,13 @@
         <v>924</v>
       </c>
       <c r="E1019" s="2" t="s">
-        <v>2125</v>
+        <v>2119</v>
       </c>
       <c r="F1019" s="2" t="s">
-        <v>2126</v>
+        <v>2120</v>
       </c>
       <c r="L1019" s="5" t="s">
-        <v>2129</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="1020" spans="1:12" x14ac:dyDescent="0.3">
@@ -24403,7 +24369,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="1066" spans="1:13" ht="30" x14ac:dyDescent="0.3">
+    <row r="1066" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1066" s="3">
         <v>3323</v>
       </c>
@@ -24417,10 +24383,10 @@
         <v>924</v>
       </c>
       <c r="E1066" s="2" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="F1066" s="4" t="s">
-        <v>2088</v>
+        <v>1855</v>
       </c>
       <c r="G1066" s="2">
         <v>50</v>
@@ -26452,10 +26418,10 @@
         <v>924</v>
       </c>
       <c r="F1200" s="2" t="s">
-        <v>2121</v>
+        <v>2115</v>
       </c>
       <c r="L1200" s="5" t="s">
-        <v>2122</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="1201" spans="1:4" x14ac:dyDescent="0.3">
@@ -27257,13 +27223,13 @@
         <v>924</v>
       </c>
       <c r="F1256" s="2" t="s">
-        <v>2093</v>
+        <v>2090</v>
       </c>
       <c r="G1256" s="2">
         <v>42</v>
       </c>
       <c r="L1256" s="5" t="s">
-        <v>2094</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="1257" spans="1:12" ht="45" x14ac:dyDescent="0.3">
@@ -27922,10 +27888,10 @@
         <v>924</v>
       </c>
       <c r="E1299" s="2" t="s">
-        <v>2120</v>
+        <v>2114</v>
       </c>
       <c r="F1299" s="2" t="s">
-        <v>2121</v>
+        <v>2115</v>
       </c>
     </row>
     <row r="1300" spans="1:12" x14ac:dyDescent="0.3">
@@ -28122,7 +28088,7 @@
         <v>924</v>
       </c>
       <c r="F1312" s="2" t="s">
-        <v>2093</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="1313" spans="1:12" x14ac:dyDescent="0.3">
@@ -29797,7 +29763,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="1423" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1423" spans="1:12" ht="30" x14ac:dyDescent="0.3">
       <c r="A1423" s="3">
         <v>6147</v>
       </c>
@@ -29813,8 +29779,8 @@
       <c r="E1423" s="2" t="s">
         <v>1924</v>
       </c>
-      <c r="F1423" s="2" t="s">
-        <v>1869</v>
+      <c r="F1423" s="4" t="s">
+        <v>2085</v>
       </c>
       <c r="G1423" s="2">
         <v>75</v>
@@ -30388,7 +30354,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="1462" spans="1:12" ht="30" x14ac:dyDescent="0.3">
+    <row r="1462" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1462" s="3">
         <v>6221</v>
       </c>
@@ -30405,13 +30371,13 @@
         <v>1884</v>
       </c>
       <c r="F1462" s="4" t="s">
-        <v>2090</v>
+        <v>1855</v>
       </c>
       <c r="G1462" s="2">
         <v>65</v>
       </c>
       <c r="L1462" s="5" t="s">
-        <v>2089</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="1463" spans="1:12" x14ac:dyDescent="0.3">
@@ -30808,7 +30774,7 @@
         <v>1693</v>
       </c>
       <c r="F1488" s="2" t="s">
-        <v>2096</v>
+        <v>2092</v>
       </c>
       <c r="G1488" s="2">
         <v>34</v>
@@ -31107,7 +31073,7 @@
         <v>1874</v>
       </c>
       <c r="L1507" s="5" t="s">
-        <v>2133</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="1508" spans="1:12" x14ac:dyDescent="0.3">
@@ -31197,16 +31163,16 @@
         <v>924</v>
       </c>
       <c r="E1513" s="2" t="s">
-        <v>2091</v>
+        <v>2088</v>
       </c>
       <c r="F1513" s="2" t="s">
-        <v>2093</v>
+        <v>2090</v>
       </c>
       <c r="G1513" s="2">
         <v>100</v>
       </c>
       <c r="L1513" s="5" t="s">
-        <v>2092</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="1514" spans="1:12" x14ac:dyDescent="0.3">
@@ -31296,7 +31262,7 @@
         <v>1782</v>
       </c>
       <c r="F1519" s="4" t="s">
-        <v>2085</v>
+        <v>1869</v>
       </c>
       <c r="G1519" s="2">
         <v>850</v>
@@ -31547,7 +31513,7 @@
         <v>1889</v>
       </c>
     </row>
-    <row r="1536" spans="1:12" ht="30" x14ac:dyDescent="0.3">
+    <row r="1536" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1536" s="3">
         <v>6538</v>
       </c>
@@ -31564,7 +31530,7 @@
         <v>1691</v>
       </c>
       <c r="F1536" s="4" t="s">
-        <v>2085</v>
+        <v>1869</v>
       </c>
       <c r="H1536" s="2">
         <v>150</v>
@@ -31680,7 +31646,7 @@
         <v>924</v>
       </c>
       <c r="F1543" s="2" t="s">
-        <v>2093</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="1544" spans="1:12" x14ac:dyDescent="0.3">
@@ -32676,7 +32642,7 @@
         <v>924</v>
       </c>
       <c r="E1609" s="2" t="s">
-        <v>2099</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="1610" spans="1:7" x14ac:dyDescent="0.3">
@@ -33070,7 +33036,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="1636" spans="1:12" ht="30" x14ac:dyDescent="0.3">
+    <row r="1636" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1636" s="3">
         <v>8299</v>
       </c>
@@ -33087,10 +33053,10 @@
         <v>1991</v>
       </c>
       <c r="F1636" s="4" t="s">
-        <v>2085</v>
+        <v>1869</v>
       </c>
       <c r="G1636" s="2">
-        <v>550</v>
+        <v>520</v>
       </c>
       <c r="L1636" s="5" t="s">
         <v>2062</v>
@@ -33161,10 +33127,10 @@
         <v>924</v>
       </c>
       <c r="E1640" s="2" t="s">
-        <v>2123</v>
+        <v>2117</v>
       </c>
       <c r="L1640" s="5" t="s">
-        <v>2124</v>
+        <v>2118</v>
       </c>
     </row>
     <row r="1641" spans="1:12" x14ac:dyDescent="0.3">
@@ -33801,10 +33767,10 @@
         <v>924</v>
       </c>
       <c r="E1684" s="2" t="s">
-        <v>2128</v>
+        <v>2122</v>
       </c>
       <c r="F1684" s="2" t="s">
-        <v>2126</v>
+        <v>2120</v>
       </c>
       <c r="G1684" s="2">
         <v>18.5</v>
@@ -33866,7 +33832,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="1689" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+    <row r="1689" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1689" s="3">
         <v>8938</v>
       </c>
@@ -33883,7 +33849,7 @@
         <v>1988</v>
       </c>
       <c r="F1689" s="4" t="s">
-        <v>2086</v>
+        <v>1869</v>
       </c>
       <c r="G1689" s="2">
         <v>60</v>
@@ -33945,7 +33911,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="1694" spans="1:7" ht="30" x14ac:dyDescent="0.3">
+    <row r="1694" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1694" s="3">
         <v>9951</v>
       </c>
@@ -33962,7 +33928,7 @@
         <v>2080</v>
       </c>
       <c r="F1694" s="4" t="s">
-        <v>2084</v>
+        <v>1855</v>
       </c>
       <c r="G1694" s="2">
         <v>90</v>

</xml_diff>

<commit_message>
update news to daily
</commit_message>
<xml_diff>
--- a/all_stock.xlsx
+++ b/all_stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\download\rich_stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B03FEC2-6719-4A33-BCEA-C9CFEAAD3E14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866AEDD5-E5DE-4EA9-883F-CFFF8558F133}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7011,7 +7011,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G113" sqref="G113"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -7022,7 +7022,7 @@
     <col min="4" max="4" width="16.75" style="2" customWidth="1"/>
     <col min="5" max="5" width="11.75" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.75" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.375" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="8.125" style="2" customWidth="1"/>
     <col min="10" max="10" width="8.125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.625" style="6" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
update 6/3 to daily
</commit_message>
<xml_diff>
--- a/all_stock.xlsx
+++ b/all_stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\download\rich_stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0544A36E-C28C-4835-AEC4-6C8C2D8BDFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DD083F-42EA-43A4-A302-C8C2E7ADFBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7080,8 +7080,8 @@
   <dimension ref="A1:N1696"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <pane ySplit="1" topLeftCell="A1343" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J1351" sqref="J1351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -24104,6 +24104,9 @@
       </c>
       <c r="I1351" s="2">
         <v>60</v>
+      </c>
+      <c r="J1351" s="2">
+        <v>75</v>
       </c>
       <c r="M1351" s="5" t="s">
         <v>1888</v>

</xml_diff>

<commit_message>
update stock daily information
</commit_message>
<xml_diff>
--- a/all_stock.xlsx
+++ b/all_stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\download\rich_stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBAE249-1671-4B74-84EC-47A742AF1A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38243CB-4B04-4285-BC63-B6CA9ABB919A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3982" uniqueCount="2006">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3988" uniqueCount="2007">
   <si>
     <t>代碼</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6522,6 +6522,11 @@
   </si>
   <si>
     <t>鋰電池</t>
+  </si>
+  <si>
+    <t>2021/7 宣布進人車用巿場
+8P 鏡頭的使用不佳(技術門檻高)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -7072,8 +7077,8 @@
   <dimension ref="A1:N1696"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A699" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H708" sqref="H708"/>
+      <pane ySplit="1" topLeftCell="A1255" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1266" sqref="F1266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -14056,7 +14061,7 @@
       <c r="D568" s="4"/>
       <c r="M568" s="7"/>
     </row>
-    <row r="569" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="569" spans="1:13" ht="30" x14ac:dyDescent="0.3">
       <c r="A569" s="3">
         <v>3008</v>
       </c>
@@ -14065,6 +14070,18 @@
       </c>
       <c r="C569" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="D569" s="2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E569" s="2" t="s">
+        <v>1994</v>
+      </c>
+      <c r="F569" s="2" t="s">
+        <v>1931</v>
+      </c>
+      <c r="M569" s="5" t="s">
+        <v>2006</v>
       </c>
     </row>
     <row r="570" spans="1:13" x14ac:dyDescent="0.3">
@@ -22461,6 +22478,12 @@
       </c>
       <c r="D1266" s="2" t="s">
         <v>1906</v>
+      </c>
+      <c r="E1266" s="2" t="s">
+        <v>1996</v>
+      </c>
+      <c r="F1266" s="2" t="s">
+        <v>1930</v>
       </c>
     </row>
     <row r="1267" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update daily information from 8/11 ~ 8/24
</commit_message>
<xml_diff>
--- a/all_stock.xlsx
+++ b/all_stock.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\download\rich_stock\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\company\rich_stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38243CB-4B04-4285-BC63-B6CA9ABB919A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B50B9A7-E05E-4FC3-87B1-E66DCD91C866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7077,8 +7077,8 @@
   <dimension ref="A1:N1696"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1255" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1266" sqref="F1266"/>
+      <pane ySplit="1" topLeftCell="A682" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G694" sqref="G694"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -15619,13 +15619,10 @@
         <v>1941</v>
       </c>
       <c r="G693" s="4">
-        <v>830</v>
+        <v>720</v>
       </c>
       <c r="H693" s="2">
-        <v>800</v>
-      </c>
-      <c r="J693" s="2">
-        <v>880</v>
+        <v>700</v>
       </c>
       <c r="K693" s="2">
         <v>1300</v>

</xml_diff>